<commit_message>
Message receiving methods rebuilding.
</commit_message>
<xml_diff>
--- a/FileTransporter/Models/Documents/Protocol commands specification.xlsx
+++ b/FileTransporter/Models/Documents/Protocol commands specification.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateu\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB75AE20-DFEA-4ED2-A9BF-5A4ECAF0C526}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="245" xr2:uid="{F5476032-7B3C-402B-BACB-3D7FBE18A503}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="12240" tabRatio="245" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Commands for client" sheetId="1" r:id="rId1"/>
     <sheet name="Commands for server" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="73">
   <si>
     <t>List of commands for client</t>
   </si>
@@ -238,14 +232,26 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>PREAMBULE</t>
+  </si>
+  <si>
+    <t>0xAA 32 times</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>10.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;zł&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -639,46 +645,6 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="9" tint="-0.24994659260841701"/>
       </left>
       <right style="medium">
@@ -835,15 +801,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -946,6 +903,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3E6CC0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3E6CC0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3E6CC0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3E6CC0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3E6CC0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3E6CC0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3E6CC0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -966,7 +972,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -999,49 +1005,67 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="29" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="33" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="32" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1083,16 +1107,22 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1107,43 +1137,52 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1155,115 +1194,103 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="25" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="31" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="32" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="33" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="21" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="29" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="29" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="29" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="30" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="21" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="20" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="30" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="26" xfId="8" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="26" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="22" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="33" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="33" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="34" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="25" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="24" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="10 % - Akcent 6" xfId="10" xr:uid="{BCF730E1-040B-4866-879D-C760719A4A09}"/>
-    <cellStyle name="10% - Akcent 1" xfId="4" xr:uid="{10043EBD-C021-4E9C-9FA6-950E2A3F928A}"/>
-    <cellStyle name="20% — akcent 1" xfId="2" builtinId="30"/>
-    <cellStyle name="20% — akcent 6" xfId="7" builtinId="50"/>
-    <cellStyle name="40% — akcent 1" xfId="3" builtinId="31"/>
-    <cellStyle name="40% — akcent 6" xfId="8" builtinId="51"/>
-    <cellStyle name="5% - Akcent 1" xfId="5" xr:uid="{2E344FBF-2AB3-4136-8F76-54178FE20127}"/>
-    <cellStyle name="60% — akcent 6" xfId="9" builtinId="52"/>
+    <cellStyle name="10 % - Akcent 6" xfId="10"/>
+    <cellStyle name="10% - Akcent 1" xfId="4"/>
+    <cellStyle name="20% - akcent 1" xfId="2" builtinId="30"/>
+    <cellStyle name="20% - akcent 6" xfId="7" builtinId="50"/>
+    <cellStyle name="40% - akcent 1" xfId="3" builtinId="31"/>
+    <cellStyle name="40% - akcent 6" xfId="8" builtinId="51"/>
+    <cellStyle name="5% - Akcent 1" xfId="5"/>
+    <cellStyle name="60% - akcent 6" xfId="9" builtinId="52"/>
     <cellStyle name="Nagłówek 1" xfId="1" builtinId="16"/>
     <cellStyle name="Nagłówek 2" xfId="6" builtinId="17"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1272,8 +1299,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF3E6CC0"/>
       <color rgb="FF547DC8"/>
-      <color rgb="FF3E6CC0"/>
       <color rgb="FFEFF6EA"/>
       <color rgb="FFF3F6FB"/>
       <color rgb="FFEDF1F9"/>
@@ -1335,7 +1362,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1387,7 +1414,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1581,236 +1608,236 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F35D557-C3EA-4ACF-8C88-33B6F0377793}">
-  <dimension ref="A1:EI14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:EI16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:AA5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:AG16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:139" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="60"/>
-      <c r="AA1" s="60"/>
-      <c r="AB1" s="60"/>
-      <c r="AC1" s="60"/>
-      <c r="AD1" s="60"/>
-      <c r="AE1" s="60"/>
-      <c r="AF1" s="60"/>
-      <c r="AG1" s="60"/>
-      <c r="AH1" s="60"/>
-      <c r="AI1" s="60"/>
-      <c r="AJ1" s="60"/>
-      <c r="AK1" s="60"/>
-      <c r="AL1" s="60"/>
-      <c r="AM1" s="60"/>
-      <c r="AN1" s="60"/>
-      <c r="AO1" s="60"/>
-      <c r="AP1" s="60"/>
-      <c r="AQ1" s="60"/>
-      <c r="AR1" s="60"/>
-      <c r="AS1" s="60"/>
-      <c r="AT1" s="60"/>
-      <c r="AU1" s="60"/>
-      <c r="AV1" s="60"/>
-      <c r="AW1" s="60"/>
-      <c r="AX1" s="60"/>
-      <c r="AY1" s="60"/>
-      <c r="AZ1" s="60"/>
-      <c r="BA1" s="60"/>
-      <c r="BB1" s="60"/>
-      <c r="BC1" s="60"/>
-      <c r="BD1" s="60"/>
-      <c r="BE1" s="60"/>
-      <c r="BF1" s="60"/>
-      <c r="BG1" s="60"/>
-      <c r="BH1" s="60"/>
-      <c r="BI1" s="60"/>
-      <c r="BJ1" s="60"/>
-      <c r="BK1" s="60"/>
-      <c r="BL1" s="60"/>
-      <c r="BM1" s="60"/>
-      <c r="BN1" s="60"/>
-      <c r="BO1" s="60"/>
-      <c r="BP1" s="60"/>
-      <c r="BQ1" s="60"/>
-      <c r="BR1" s="60"/>
-      <c r="BS1" s="60"/>
-      <c r="BT1" s="60"/>
-      <c r="BU1" s="60"/>
-      <c r="BV1" s="60"/>
-      <c r="BW1" s="60"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="71"/>
+      <c r="X1" s="71"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="71"/>
+      <c r="AA1" s="71"/>
+      <c r="AB1" s="71"/>
+      <c r="AC1" s="71"/>
+      <c r="AD1" s="71"/>
+      <c r="AE1" s="71"/>
+      <c r="AF1" s="71"/>
+      <c r="AG1" s="71"/>
+      <c r="AH1" s="71"/>
+      <c r="AI1" s="71"/>
+      <c r="AJ1" s="71"/>
+      <c r="AK1" s="71"/>
+      <c r="AL1" s="71"/>
+      <c r="AM1" s="71"/>
+      <c r="AN1" s="71"/>
+      <c r="AO1" s="71"/>
+      <c r="AP1" s="71"/>
+      <c r="AQ1" s="71"/>
+      <c r="AR1" s="71"/>
+      <c r="AS1" s="71"/>
+      <c r="AT1" s="71"/>
+      <c r="AU1" s="71"/>
+      <c r="AV1" s="71"/>
+      <c r="AW1" s="71"/>
+      <c r="AX1" s="71"/>
+      <c r="AY1" s="71"/>
+      <c r="AZ1" s="71"/>
+      <c r="BA1" s="71"/>
+      <c r="BB1" s="71"/>
+      <c r="BC1" s="71"/>
+      <c r="BD1" s="71"/>
+      <c r="BE1" s="71"/>
+      <c r="BF1" s="71"/>
+      <c r="BG1" s="71"/>
+      <c r="BH1" s="71"/>
+      <c r="BI1" s="71"/>
+      <c r="BJ1" s="71"/>
+      <c r="BK1" s="71"/>
+      <c r="BL1" s="71"/>
+      <c r="BM1" s="71"/>
+      <c r="BN1" s="71"/>
+      <c r="BO1" s="71"/>
+      <c r="BP1" s="71"/>
+      <c r="BQ1" s="71"/>
+      <c r="BR1" s="71"/>
+      <c r="BS1" s="71"/>
+      <c r="BT1" s="71"/>
+      <c r="BU1" s="71"/>
+      <c r="BV1" s="71"/>
+      <c r="BW1" s="71"/>
     </row>
-    <row r="2" spans="1:139" s="92" customFormat="1" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+    <row r="2" spans="1:139" s="27" customFormat="1" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="89" t="s">
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="90"/>
-      <c r="S2" s="90"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="90"/>
-      <c r="W2" s="90"/>
-      <c r="X2" s="90"/>
-      <c r="Y2" s="90"/>
-      <c r="Z2" s="90"/>
-      <c r="AA2" s="90"/>
-      <c r="AB2" s="90"/>
-      <c r="AC2" s="90"/>
-      <c r="AD2" s="90"/>
-      <c r="AE2" s="90"/>
-      <c r="AF2" s="90"/>
-      <c r="AG2" s="90"/>
-      <c r="AH2" s="90"/>
-      <c r="AI2" s="90"/>
-      <c r="AJ2" s="90"/>
-      <c r="AK2" s="90"/>
-      <c r="AL2" s="90"/>
-      <c r="AM2" s="90"/>
-      <c r="AN2" s="90"/>
-      <c r="AO2" s="90"/>
-      <c r="AP2" s="90"/>
-      <c r="AQ2" s="90"/>
-      <c r="AR2" s="90"/>
-      <c r="AS2" s="90"/>
-      <c r="AT2" s="90"/>
-      <c r="AU2" s="90"/>
-      <c r="AV2" s="90"/>
-      <c r="AW2" s="90"/>
-      <c r="AX2" s="90"/>
-      <c r="AY2" s="90"/>
-      <c r="AZ2" s="90"/>
-      <c r="BA2" s="90"/>
-      <c r="BB2" s="90"/>
-      <c r="BC2" s="90"/>
-      <c r="BD2" s="90"/>
-      <c r="BE2" s="90"/>
-      <c r="BF2" s="90"/>
-      <c r="BG2" s="90"/>
-      <c r="BH2" s="90"/>
-      <c r="BI2" s="90"/>
-      <c r="BJ2" s="90"/>
-      <c r="BK2" s="90"/>
-      <c r="BL2" s="90"/>
-      <c r="BM2" s="90"/>
-      <c r="BN2" s="90"/>
-      <c r="BO2" s="90"/>
-      <c r="BP2" s="90"/>
-      <c r="BQ2" s="90"/>
-      <c r="BR2" s="90"/>
-      <c r="BS2" s="90"/>
-      <c r="BT2" s="90"/>
-      <c r="BU2" s="90"/>
-      <c r="BV2" s="90"/>
-      <c r="BW2" s="91"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="64"/>
+      <c r="S2" s="64"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="64"/>
+      <c r="V2" s="64"/>
+      <c r="W2" s="64"/>
+      <c r="X2" s="64"/>
+      <c r="Y2" s="64"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
+      <c r="AC2" s="64"/>
+      <c r="AD2" s="64"/>
+      <c r="AE2" s="64"/>
+      <c r="AF2" s="64"/>
+      <c r="AG2" s="64"/>
+      <c r="AH2" s="64"/>
+      <c r="AI2" s="64"/>
+      <c r="AJ2" s="64"/>
+      <c r="AK2" s="64"/>
+      <c r="AL2" s="64"/>
+      <c r="AM2" s="64"/>
+      <c r="AN2" s="64"/>
+      <c r="AO2" s="64"/>
+      <c r="AP2" s="64"/>
+      <c r="AQ2" s="64"/>
+      <c r="AR2" s="64"/>
+      <c r="AS2" s="64"/>
+      <c r="AT2" s="64"/>
+      <c r="AU2" s="64"/>
+      <c r="AV2" s="64"/>
+      <c r="AW2" s="64"/>
+      <c r="AX2" s="64"/>
+      <c r="AY2" s="64"/>
+      <c r="AZ2" s="64"/>
+      <c r="BA2" s="64"/>
+      <c r="BB2" s="64"/>
+      <c r="BC2" s="64"/>
+      <c r="BD2" s="64"/>
+      <c r="BE2" s="64"/>
+      <c r="BF2" s="64"/>
+      <c r="BG2" s="64"/>
+      <c r="BH2" s="64"/>
+      <c r="BI2" s="64"/>
+      <c r="BJ2" s="64"/>
+      <c r="BK2" s="64"/>
+      <c r="BL2" s="64"/>
+      <c r="BM2" s="64"/>
+      <c r="BN2" s="64"/>
+      <c r="BO2" s="64"/>
+      <c r="BP2" s="64"/>
+      <c r="BQ2" s="64"/>
+      <c r="BR2" s="64"/>
+      <c r="BS2" s="64"/>
+      <c r="BT2" s="64"/>
+      <c r="BU2" s="64"/>
+      <c r="BV2" s="64"/>
+      <c r="BW2" s="65"/>
     </row>
     <row r="3" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="50" t="s">
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51" t="s">
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
-      <c r="U3" s="51"/>
-      <c r="V3" s="51"/>
-      <c r="W3" s="51"/>
-      <c r="X3" s="51"/>
-      <c r="Y3" s="51"/>
-      <c r="Z3" s="51" t="s">
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="AA3" s="51"/>
-      <c r="AB3" s="51"/>
-      <c r="AC3" s="51"/>
-      <c r="AD3" s="51"/>
-      <c r="AE3" s="51"/>
-      <c r="AF3" s="51" t="s">
+      <c r="AA3" s="49"/>
+      <c r="AB3" s="49"/>
+      <c r="AC3" s="49"/>
+      <c r="AD3" s="49"/>
+      <c r="AE3" s="49"/>
+      <c r="AF3" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="AG3" s="51"/>
-      <c r="AH3" s="51"/>
-      <c r="AI3" s="51"/>
-      <c r="AJ3" s="51"/>
-      <c r="AK3" s="51"/>
-      <c r="AL3" s="51"/>
-      <c r="AM3" s="53"/>
+      <c r="AG3" s="49"/>
+      <c r="AH3" s="49"/>
+      <c r="AI3" s="49"/>
+      <c r="AJ3" s="49"/>
+      <c r="AK3" s="49"/>
+      <c r="AL3" s="49"/>
+      <c r="AM3" s="56"/>
       <c r="AN3" s="3"/>
       <c r="AO3" s="3"/>
       <c r="AP3" s="3"/>
@@ -1847,30 +1874,30 @@
       <c r="BU3" s="3"/>
     </row>
     <row r="4" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="24" t="s">
+      <c r="A4" s="32"/>
+      <c r="B4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="13" t="s">
+      <c r="H4" s="61"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="12" t="s">
         <v>16</v>
       </c>
       <c r="M4" s="9" t="s">
@@ -1882,20 +1909,20 @@
       <c r="O4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q4" s="52" t="s">
+      <c r="P4" s="99" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="R4" s="52"/>
-      <c r="S4" s="52"/>
-      <c r="T4" s="52"/>
-      <c r="U4" s="52"/>
-      <c r="V4" s="52"/>
-      <c r="W4" s="52"/>
-      <c r="X4" s="52"/>
-      <c r="Y4" s="52"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="50"/>
+      <c r="U4" s="50"/>
+      <c r="V4" s="50"/>
+      <c r="W4" s="50"/>
+      <c r="X4" s="50"/>
+      <c r="Y4" s="50"/>
       <c r="Z4" s="9" t="s">
         <v>15</v>
       </c>
@@ -1911,19 +1938,19 @@
       <c r="AD4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AE4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF4" s="52" t="s">
+      <c r="AE4" s="99" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF4" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="AG4" s="52"/>
-      <c r="AH4" s="52"/>
-      <c r="AI4" s="52"/>
-      <c r="AJ4" s="52"/>
-      <c r="AK4" s="52"/>
-      <c r="AL4" s="52"/>
-      <c r="AM4" s="54"/>
+      <c r="AG4" s="50"/>
+      <c r="AH4" s="50"/>
+      <c r="AI4" s="50"/>
+      <c r="AJ4" s="50"/>
+      <c r="AK4" s="50"/>
+      <c r="AL4" s="50"/>
+      <c r="AM4" s="57"/>
       <c r="AN4" s="5"/>
       <c r="AO4" s="5"/>
       <c r="AP4" s="3"/>
@@ -1960,71 +1987,71 @@
       <c r="BU4" s="3"/>
     </row>
     <row r="5" spans="1:139" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="32" t="s">
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="32"/>
-      <c r="T5" s="32"/>
-      <c r="U5" s="32"/>
-      <c r="V5" s="32"/>
-      <c r="W5" s="32"/>
-      <c r="X5" s="32"/>
-      <c r="Y5" s="32"/>
-      <c r="Z5" s="32"/>
-      <c r="AA5" s="32"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
+      <c r="W5" s="38"/>
+      <c r="X5" s="38"/>
+      <c r="Y5" s="38"/>
+      <c r="Z5" s="38"/>
+      <c r="AA5" s="38"/>
       <c r="AB5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="AC5" s="32" t="s">
+      <c r="AC5" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="AD5" s="32"/>
-      <c r="AE5" s="32"/>
-      <c r="AF5" s="32"/>
-      <c r="AG5" s="32"/>
-      <c r="AH5" s="32"/>
-      <c r="AI5" s="32"/>
-      <c r="AJ5" s="32"/>
-      <c r="AK5" s="32"/>
-      <c r="AL5" s="32"/>
-      <c r="AM5" s="30" t="s">
+      <c r="AD5" s="38"/>
+      <c r="AE5" s="38"/>
+      <c r="AF5" s="38"/>
+      <c r="AG5" s="38"/>
+      <c r="AH5" s="38"/>
+      <c r="AI5" s="38"/>
+      <c r="AJ5" s="38"/>
+      <c r="AK5" s="38"/>
+      <c r="AL5" s="38"/>
+      <c r="AM5" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="AN5" s="31"/>
-      <c r="AO5" s="33" t="s">
+      <c r="AN5" s="37"/>
+      <c r="AO5" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="AP5" s="34"/>
-      <c r="AQ5" s="34"/>
-      <c r="AR5" s="34"/>
-      <c r="AS5" s="34"/>
-      <c r="AT5" s="34"/>
-      <c r="AU5" s="34"/>
-      <c r="AV5" s="35"/>
+      <c r="AP5" s="40"/>
+      <c r="AQ5" s="40"/>
+      <c r="AR5" s="40"/>
+      <c r="AS5" s="40"/>
+      <c r="AT5" s="40"/>
+      <c r="AU5" s="40"/>
+      <c r="AV5" s="41"/>
     </row>
     <row r="6" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="7" t="s">
         <v>26</v>
       </c>
@@ -2052,91 +2079,91 @@
       <c r="J6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="43"/>
-      <c r="L6" s="32" t="s">
+      <c r="K6" s="47"/>
+      <c r="L6" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="32"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
-      <c r="W6" s="32"/>
-      <c r="X6" s="32"/>
-      <c r="Y6" s="32"/>
-      <c r="Z6" s="32"/>
-      <c r="AA6" s="32"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="38"/>
+      <c r="V6" s="38"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="38"/>
+      <c r="Z6" s="38"/>
+      <c r="AA6" s="38"/>
       <c r="AB6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AC6" s="32" t="s">
+      <c r="AC6" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="AD6" s="32"/>
-      <c r="AE6" s="32"/>
-      <c r="AF6" s="32"/>
-      <c r="AG6" s="32"/>
-      <c r="AH6" s="32"/>
-      <c r="AI6" s="32"/>
-      <c r="AJ6" s="32"/>
-      <c r="AK6" s="32"/>
-      <c r="AL6" s="32"/>
+      <c r="AD6" s="38"/>
+      <c r="AE6" s="38"/>
+      <c r="AF6" s="38"/>
+      <c r="AG6" s="38"/>
+      <c r="AH6" s="38"/>
+      <c r="AI6" s="38"/>
+      <c r="AJ6" s="38"/>
+      <c r="AK6" s="38"/>
+      <c r="AL6" s="38"/>
       <c r="AM6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AN6" s="18" t="s">
+      <c r="AN6" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="AO6" s="33" t="s">
+      <c r="AO6" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="AP6" s="34"/>
-      <c r="AQ6" s="34"/>
-      <c r="AR6" s="34"/>
-      <c r="AS6" s="34"/>
-      <c r="AT6" s="34"/>
-      <c r="AU6" s="34"/>
-      <c r="AV6" s="35"/>
+      <c r="AP6" s="40"/>
+      <c r="AQ6" s="40"/>
+      <c r="AR6" s="40"/>
+      <c r="AS6" s="40"/>
+      <c r="AT6" s="40"/>
+      <c r="AU6" s="40"/>
+      <c r="AV6" s="41"/>
     </row>
     <row r="7" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
-      <c r="L7" s="32" t="s">
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="32"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="32"/>
-      <c r="V7" s="32"/>
-      <c r="W7" s="32"/>
-      <c r="X7" s="32"/>
-      <c r="Y7" s="32"/>
-      <c r="Z7" s="32"/>
-      <c r="AA7" s="39"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="38"/>
+      <c r="T7" s="38"/>
+      <c r="U7" s="38"/>
+      <c r="V7" s="38"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="38"/>
+      <c r="Y7" s="38"/>
+      <c r="Z7" s="38"/>
+      <c r="AA7" s="45"/>
       <c r="AB7" s="4"/>
       <c r="AC7" s="4"/>
       <c r="AD7" s="4"/>
@@ -2251,7 +2278,7 @@
       <c r="EI7" s="1"/>
     </row>
     <row r="8" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="7" t="s">
         <v>49</v>
       </c>
@@ -2282,24 +2309,24 @@
       <c r="K8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="32" t="s">
+      <c r="L8" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="32"/>
-      <c r="U8" s="32"/>
-      <c r="V8" s="32"/>
-      <c r="W8" s="32"/>
-      <c r="X8" s="32"/>
-      <c r="Y8" s="32"/>
-      <c r="Z8" s="32"/>
-      <c r="AA8" s="39"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="38"/>
+      <c r="T8" s="38"/>
+      <c r="U8" s="38"/>
+      <c r="V8" s="38"/>
+      <c r="W8" s="38"/>
+      <c r="X8" s="38"/>
+      <c r="Y8" s="38"/>
+      <c r="Z8" s="38"/>
+      <c r="AA8" s="45"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
       <c r="AD8" s="4"/>
@@ -2414,104 +2441,104 @@
       <c r="EI8" s="1"/>
     </row>
     <row r="9" spans="1:139" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="33" t="s">
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
-      <c r="T9" s="34"/>
-      <c r="U9" s="34"/>
-      <c r="V9" s="34"/>
-      <c r="W9" s="34"/>
-      <c r="X9" s="34"/>
-      <c r="Y9" s="34"/>
-      <c r="Z9" s="34"/>
-      <c r="AA9" s="62"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="40"/>
+      <c r="V9" s="40"/>
+      <c r="W9" s="40"/>
+      <c r="X9" s="40"/>
+      <c r="Y9" s="40"/>
+      <c r="Z9" s="40"/>
+      <c r="AA9" s="73"/>
       <c r="AB9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AC9" s="32" t="s">
+      <c r="AC9" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="AD9" s="32"/>
-      <c r="AE9" s="32"/>
-      <c r="AF9" s="32"/>
-      <c r="AG9" s="32"/>
-      <c r="AH9" s="32"/>
-      <c r="AI9" s="32"/>
-      <c r="AJ9" s="32"/>
-      <c r="AK9" s="32" t="s">
+      <c r="AD9" s="38"/>
+      <c r="AE9" s="38"/>
+      <c r="AF9" s="38"/>
+      <c r="AG9" s="38"/>
+      <c r="AH9" s="38"/>
+      <c r="AI9" s="38"/>
+      <c r="AJ9" s="38"/>
+      <c r="AK9" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="AL9" s="32"/>
-      <c r="AM9" s="32"/>
-      <c r="AN9" s="32"/>
-      <c r="AO9" s="32"/>
-      <c r="AP9" s="32"/>
-      <c r="AQ9" s="32"/>
-      <c r="AR9" s="32"/>
+      <c r="AL9" s="38"/>
+      <c r="AM9" s="38"/>
+      <c r="AN9" s="38"/>
+      <c r="AO9" s="38"/>
+      <c r="AP9" s="38"/>
+      <c r="AQ9" s="38"/>
+      <c r="AR9" s="38"/>
       <c r="AS9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="AT9" s="32" t="s">
+      <c r="AT9" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="AU9" s="32"/>
-      <c r="AV9" s="32"/>
-      <c r="AW9" s="32"/>
-      <c r="AX9" s="32"/>
-      <c r="AY9" s="32"/>
-      <c r="AZ9" s="32"/>
-      <c r="BA9" s="32"/>
-      <c r="BB9" s="32"/>
+      <c r="AU9" s="38"/>
+      <c r="AV9" s="38"/>
+      <c r="AW9" s="38"/>
+      <c r="AX9" s="38"/>
+      <c r="AY9" s="38"/>
+      <c r="AZ9" s="38"/>
+      <c r="BA9" s="38"/>
+      <c r="BB9" s="38"/>
       <c r="BC9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="BD9" s="33" t="s">
+      <c r="BD9" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="BE9" s="34"/>
-      <c r="BF9" s="34"/>
-      <c r="BG9" s="34"/>
-      <c r="BH9" s="34"/>
-      <c r="BI9" s="34"/>
-      <c r="BJ9" s="34"/>
-      <c r="BK9" s="34"/>
-      <c r="BL9" s="34"/>
-      <c r="BM9" s="34"/>
-      <c r="BN9" s="34"/>
-      <c r="BO9" s="34"/>
-      <c r="BP9" s="34"/>
-      <c r="BQ9" s="34"/>
-      <c r="BR9" s="34"/>
-      <c r="BS9" s="34"/>
-      <c r="BT9" s="34"/>
-      <c r="BU9" s="34"/>
-      <c r="BV9" s="34"/>
-      <c r="BW9" s="35"/>
+      <c r="BE9" s="40"/>
+      <c r="BF9" s="40"/>
+      <c r="BG9" s="40"/>
+      <c r="BH9" s="40"/>
+      <c r="BI9" s="40"/>
+      <c r="BJ9" s="40"/>
+      <c r="BK9" s="40"/>
+      <c r="BL9" s="40"/>
+      <c r="BM9" s="40"/>
+      <c r="BN9" s="40"/>
+      <c r="BO9" s="40"/>
+      <c r="BP9" s="40"/>
+      <c r="BQ9" s="40"/>
+      <c r="BR9" s="40"/>
+      <c r="BS9" s="40"/>
+      <c r="BT9" s="40"/>
+      <c r="BU9" s="40"/>
+      <c r="BV9" s="40"/>
+      <c r="BW9" s="41"/>
     </row>
     <row r="10" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="7" t="s">
         <v>49</v>
       </c>
@@ -2539,124 +2566,124 @@
       <c r="J10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="K10" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="33" t="s">
+      <c r="L10" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
-      <c r="T10" s="34"/>
-      <c r="U10" s="34"/>
-      <c r="V10" s="34"/>
-      <c r="W10" s="34"/>
-      <c r="X10" s="34"/>
-      <c r="Y10" s="34"/>
-      <c r="Z10" s="34"/>
-      <c r="AA10" s="62"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="40"/>
+      <c r="S10" s="40"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="40"/>
+      <c r="V10" s="40"/>
+      <c r="W10" s="40"/>
+      <c r="X10" s="40"/>
+      <c r="Y10" s="40"/>
+      <c r="Z10" s="40"/>
+      <c r="AA10" s="73"/>
       <c r="AB10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AC10" s="32" t="s">
+      <c r="AC10" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="AD10" s="32"/>
-      <c r="AE10" s="32"/>
-      <c r="AF10" s="32"/>
-      <c r="AG10" s="32"/>
-      <c r="AH10" s="32"/>
-      <c r="AI10" s="32"/>
-      <c r="AJ10" s="32"/>
-      <c r="AK10" s="32" t="s">
+      <c r="AD10" s="38"/>
+      <c r="AE10" s="38"/>
+      <c r="AF10" s="38"/>
+      <c r="AG10" s="38"/>
+      <c r="AH10" s="38"/>
+      <c r="AI10" s="38"/>
+      <c r="AJ10" s="38"/>
+      <c r="AK10" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="AL10" s="32"/>
-      <c r="AM10" s="32"/>
-      <c r="AN10" s="32"/>
-      <c r="AO10" s="32"/>
-      <c r="AP10" s="32"/>
-      <c r="AQ10" s="32"/>
-      <c r="AR10" s="32"/>
+      <c r="AL10" s="38"/>
+      <c r="AM10" s="38"/>
+      <c r="AN10" s="38"/>
+      <c r="AO10" s="38"/>
+      <c r="AP10" s="38"/>
+      <c r="AQ10" s="38"/>
+      <c r="AR10" s="38"/>
       <c r="AS10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AT10" s="32" t="s">
+      <c r="AT10" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="AU10" s="32"/>
-      <c r="AV10" s="32"/>
-      <c r="AW10" s="32"/>
-      <c r="AX10" s="32"/>
-      <c r="AY10" s="32"/>
-      <c r="AZ10" s="32"/>
-      <c r="BA10" s="32"/>
-      <c r="BB10" s="32"/>
+      <c r="AU10" s="38"/>
+      <c r="AV10" s="38"/>
+      <c r="AW10" s="38"/>
+      <c r="AX10" s="38"/>
+      <c r="AY10" s="38"/>
+      <c r="AZ10" s="38"/>
+      <c r="BA10" s="38"/>
+      <c r="BB10" s="38"/>
       <c r="BC10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="BD10" s="33" t="s">
+      <c r="BD10" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="BE10" s="34"/>
-      <c r="BF10" s="34"/>
-      <c r="BG10" s="34"/>
-      <c r="BH10" s="34"/>
-      <c r="BI10" s="34"/>
-      <c r="BJ10" s="34"/>
-      <c r="BK10" s="34"/>
-      <c r="BL10" s="34"/>
-      <c r="BM10" s="34"/>
-      <c r="BN10" s="34"/>
-      <c r="BO10" s="34"/>
-      <c r="BP10" s="34"/>
-      <c r="BQ10" s="34"/>
-      <c r="BR10" s="34"/>
-      <c r="BS10" s="34"/>
-      <c r="BT10" s="34"/>
-      <c r="BU10" s="34"/>
-      <c r="BV10" s="34"/>
-      <c r="BW10" s="35"/>
+      <c r="BE10" s="40"/>
+      <c r="BF10" s="40"/>
+      <c r="BG10" s="40"/>
+      <c r="BH10" s="40"/>
+      <c r="BI10" s="40"/>
+      <c r="BJ10" s="40"/>
+      <c r="BK10" s="40"/>
+      <c r="BL10" s="40"/>
+      <c r="BM10" s="40"/>
+      <c r="BN10" s="40"/>
+      <c r="BO10" s="40"/>
+      <c r="BP10" s="40"/>
+      <c r="BQ10" s="40"/>
+      <c r="BR10" s="40"/>
+      <c r="BS10" s="40"/>
+      <c r="BT10" s="40"/>
+      <c r="BU10" s="40"/>
+      <c r="BV10" s="40"/>
+      <c r="BW10" s="41"/>
     </row>
     <row r="11" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="32" t="s">
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="32"/>
-      <c r="S11" s="32"/>
-      <c r="T11" s="32"/>
-      <c r="U11" s="32"/>
-      <c r="V11" s="32"/>
-      <c r="W11" s="32"/>
-      <c r="X11" s="32"/>
-      <c r="Y11" s="32"/>
-      <c r="Z11" s="32"/>
-      <c r="AA11" s="39"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="38"/>
+      <c r="T11" s="38"/>
+      <c r="U11" s="38"/>
+      <c r="V11" s="38"/>
+      <c r="W11" s="38"/>
+      <c r="X11" s="38"/>
+      <c r="Y11" s="38"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="45"/>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
@@ -2705,7 +2732,7 @@
       <c r="BU11" s="3"/>
     </row>
     <row r="12" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
@@ -2727,27 +2754,27 @@
       <c r="H12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="27"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="32" t="s">
+      <c r="I12" s="33"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="32"/>
-      <c r="S12" s="32"/>
-      <c r="T12" s="32"/>
-      <c r="U12" s="32"/>
-      <c r="V12" s="32"/>
-      <c r="W12" s="32"/>
-      <c r="X12" s="32"/>
-      <c r="Y12" s="32"/>
-      <c r="Z12" s="32"/>
-      <c r="AA12" s="39"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="38"/>
+      <c r="T12" s="38"/>
+      <c r="U12" s="38"/>
+      <c r="V12" s="38"/>
+      <c r="W12" s="38"/>
+      <c r="X12" s="38"/>
+      <c r="Y12" s="38"/>
+      <c r="Z12" s="38"/>
+      <c r="AA12" s="45"/>
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
@@ -2796,83 +2823,167 @@
       <c r="BU12" s="3"/>
     </row>
     <row r="13" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="32" t="s">
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32"/>
-      <c r="V13" s="32"/>
-      <c r="W13" s="32"/>
-      <c r="X13" s="32"/>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="32"/>
-      <c r="AA13" s="39"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="38"/>
+      <c r="T13" s="38"/>
+      <c r="U13" s="38"/>
+      <c r="V13" s="38"/>
+      <c r="W13" s="38"/>
+      <c r="X13" s="38"/>
+      <c r="Y13" s="38"/>
+      <c r="Z13" s="38"/>
+      <c r="AA13" s="45"/>
     </row>
     <row r="14" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="12" t="s">
+      <c r="A14" s="32"/>
+      <c r="B14" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="32" t="s">
+      <c r="G14" s="33"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
-      <c r="T14" s="32"/>
-      <c r="U14" s="32"/>
-      <c r="V14" s="32"/>
-      <c r="W14" s="32"/>
-      <c r="X14" s="32"/>
-      <c r="Y14" s="32"/>
-      <c r="Z14" s="32"/>
-      <c r="AA14" s="39"/>
+      <c r="M14" s="101"/>
+      <c r="N14" s="101"/>
+      <c r="O14" s="101"/>
+      <c r="P14" s="101"/>
+      <c r="Q14" s="101"/>
+      <c r="R14" s="101"/>
+      <c r="S14" s="101"/>
+      <c r="T14" s="101"/>
+      <c r="U14" s="101"/>
+      <c r="V14" s="101"/>
+      <c r="W14" s="101"/>
+      <c r="X14" s="101"/>
+      <c r="Y14" s="101"/>
+      <c r="Z14" s="101"/>
+      <c r="AA14" s="102"/>
+    </row>
+    <row r="15" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="30"/>
+      <c r="V15" s="30"/>
+      <c r="W15" s="30"/>
+      <c r="X15" s="30"/>
+      <c r="Y15" s="30"/>
+      <c r="Z15" s="30"/>
+      <c r="AA15" s="30"/>
+      <c r="AB15" s="30"/>
+      <c r="AC15" s="30"/>
+      <c r="AD15" s="30"/>
+      <c r="AE15" s="30"/>
+      <c r="AF15" s="30"/>
+      <c r="AG15" s="31"/>
+    </row>
+    <row r="16" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="30"/>
+      <c r="Z16" s="30"/>
+      <c r="AA16" s="30"/>
+      <c r="AB16" s="30"/>
+      <c r="AC16" s="30"/>
+      <c r="AD16" s="30"/>
+      <c r="AE16" s="30"/>
+      <c r="AF16" s="30"/>
+      <c r="AG16" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="51">
+    <mergeCell ref="BD9:BW9"/>
+    <mergeCell ref="BD10:BW10"/>
+    <mergeCell ref="AC5:AL5"/>
+    <mergeCell ref="B16:AG16"/>
+    <mergeCell ref="B15:AG15"/>
+    <mergeCell ref="L2:BW2"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:G3"/>
     <mergeCell ref="A1:BW1"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:F13"/>
@@ -2886,20 +2997,6 @@
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="L13:AA13"/>
     <mergeCell ref="L14:AA14"/>
-    <mergeCell ref="BD9:BW9"/>
-    <mergeCell ref="BD10:BW10"/>
-    <mergeCell ref="AC5:AL5"/>
-    <mergeCell ref="Z3:AE3"/>
-    <mergeCell ref="AF3:AM3"/>
-    <mergeCell ref="AF4:AM4"/>
-    <mergeCell ref="H3:K4"/>
-    <mergeCell ref="L2:BW2"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="Q3:Y3"/>
-    <mergeCell ref="Q4:Y4"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="A9:A10"/>
@@ -2907,6 +3004,16 @@
     <mergeCell ref="L12:AA12"/>
     <mergeCell ref="B9:K9"/>
     <mergeCell ref="I11:K12"/>
+    <mergeCell ref="AT10:BB10"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="Q3:Y3"/>
+    <mergeCell ref="Q4:Y4"/>
+    <mergeCell ref="Z3:AE3"/>
+    <mergeCell ref="AF3:AM3"/>
+    <mergeCell ref="AF4:AM4"/>
+    <mergeCell ref="H3:K4"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="G13:K14"/>
     <mergeCell ref="AM5:AN5"/>
     <mergeCell ref="AC9:AJ9"/>
@@ -2920,20 +3027,19 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="AC6:AL6"/>
     <mergeCell ref="AT9:BB9"/>
-    <mergeCell ref="AT10:BB10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6735471A-DB2C-4E21-A01F-06623F4173F6}">
-  <dimension ref="A1:AX20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AX22"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="AX15" sqref="AX15:AX17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AG26" sqref="AG26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2944,614 +3050,693 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="69"/>
-      <c r="X1" s="69"/>
-      <c r="Y1" s="69"/>
-      <c r="Z1" s="69"/>
-      <c r="AA1" s="69"/>
-      <c r="AB1" s="69"/>
-      <c r="AC1" s="69"/>
-      <c r="AD1" s="69"/>
-      <c r="AE1" s="69"/>
-      <c r="AF1" s="69"/>
-      <c r="AG1" s="69"/>
-      <c r="AH1" s="69"/>
-      <c r="AI1" s="69"/>
-      <c r="AJ1" s="69"/>
-      <c r="AK1" s="69"/>
-      <c r="AL1" s="69"/>
-      <c r="AM1" s="69"/>
-      <c r="AN1" s="69"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="80"/>
+      <c r="AA1" s="80"/>
+      <c r="AB1" s="80"/>
+      <c r="AC1" s="80"/>
+      <c r="AD1" s="80"/>
+      <c r="AE1" s="80"/>
+      <c r="AF1" s="80"/>
+      <c r="AG1" s="80"/>
+      <c r="AH1" s="80"/>
+      <c r="AI1" s="80"/>
+      <c r="AJ1" s="80"/>
+      <c r="AK1" s="80"/>
+      <c r="AL1" s="80"/>
+      <c r="AM1" s="80"/>
+      <c r="AN1" s="80"/>
     </row>
     <row r="2" spans="1:50" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67" t="s">
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="67"/>
-      <c r="S2" s="67"/>
-      <c r="T2" s="67"/>
-      <c r="U2" s="67"/>
-      <c r="V2" s="67"/>
-      <c r="W2" s="67"/>
-      <c r="X2" s="67"/>
-      <c r="Y2" s="67"/>
-      <c r="Z2" s="67"/>
-      <c r="AA2" s="67"/>
-      <c r="AB2" s="67"/>
-      <c r="AC2" s="67"/>
-      <c r="AD2" s="67"/>
-      <c r="AE2" s="67"/>
-      <c r="AF2" s="67"/>
-      <c r="AG2" s="67"/>
-      <c r="AH2" s="67"/>
-      <c r="AI2" s="67"/>
-      <c r="AJ2" s="67"/>
-      <c r="AK2" s="67"/>
-      <c r="AL2" s="67"/>
-      <c r="AM2" s="67"/>
-      <c r="AN2" s="67"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
+      <c r="V2" s="78"/>
+      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
+      <c r="Y2" s="78"/>
+      <c r="Z2" s="78"/>
+      <c r="AA2" s="78"/>
+      <c r="AB2" s="78"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="78"/>
+      <c r="AE2" s="78"/>
+      <c r="AF2" s="78"/>
+      <c r="AG2" s="78"/>
+      <c r="AH2" s="78"/>
+      <c r="AI2" s="78"/>
+      <c r="AJ2" s="78"/>
+      <c r="AK2" s="78"/>
+      <c r="AL2" s="78"/>
+      <c r="AM2" s="78"/>
+      <c r="AN2" s="78"/>
     </row>
     <row r="3" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="84" t="s">
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="84"/>
-      <c r="S3" s="84"/>
-      <c r="T3" s="84"/>
-      <c r="U3" s="84"/>
-      <c r="V3" s="84"/>
-      <c r="W3" s="84"/>
-      <c r="X3" s="84"/>
-      <c r="Y3" s="84"/>
-      <c r="Z3" s="84"/>
-      <c r="AA3" s="84"/>
-      <c r="AB3" s="84"/>
-      <c r="AC3" s="84"/>
-      <c r="AD3" s="84"/>
-      <c r="AE3" s="84"/>
-      <c r="AF3" s="85"/>
+      <c r="R3" s="83"/>
+      <c r="S3" s="83"/>
+      <c r="T3" s="83"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="83"/>
+      <c r="W3" s="83"/>
+      <c r="X3" s="83"/>
+      <c r="Y3" s="83"/>
+      <c r="Z3" s="83"/>
+      <c r="AA3" s="83"/>
+      <c r="AB3" s="83"/>
+      <c r="AC3" s="83"/>
+      <c r="AD3" s="83"/>
+      <c r="AE3" s="83"/>
+      <c r="AF3" s="84"/>
     </row>
     <row r="4" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="75"/>
+      <c r="B4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="75"/>
-      <c r="L4" s="76"/>
-      <c r="M4" s="76"/>
-      <c r="N4" s="76"/>
-      <c r="O4" s="76"/>
-      <c r="P4" s="77"/>
-      <c r="Q4" s="86" t="s">
+      <c r="K4" s="93"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="94"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="86"/>
-      <c r="AD4" s="86"/>
-      <c r="AE4" s="86"/>
-      <c r="AF4" s="87"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="85"/>
+      <c r="V4" s="85"/>
+      <c r="W4" s="85"/>
+      <c r="X4" s="85"/>
+      <c r="Y4" s="85"/>
+      <c r="Z4" s="85"/>
+      <c r="AA4" s="85"/>
+      <c r="AB4" s="85"/>
+      <c r="AC4" s="85"/>
+      <c r="AD4" s="85"/>
+      <c r="AE4" s="85"/>
+      <c r="AF4" s="86"/>
     </row>
     <row r="5" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="64"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="75"/>
+      <c r="B6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="64"/>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="75"/>
+      <c r="B8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="76"/>
-      <c r="M9" s="76"/>
-      <c r="N9" s="76"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="77"/>
-      <c r="Q9" s="70" t="s">
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="94"/>
+      <c r="K9" s="94"/>
+      <c r="L9" s="94"/>
+      <c r="M9" s="94"/>
+      <c r="N9" s="94"/>
+      <c r="O9" s="94"/>
+      <c r="P9" s="95"/>
+      <c r="Q9" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="R9" s="70"/>
-      <c r="S9" s="70"/>
-      <c r="T9" s="70"/>
-      <c r="U9" s="70"/>
-      <c r="V9" s="70"/>
-      <c r="W9" s="70"/>
-      <c r="X9" s="70"/>
-      <c r="Y9" s="70"/>
-      <c r="Z9" s="70"/>
-      <c r="AA9" s="70"/>
-      <c r="AB9" s="70"/>
-      <c r="AC9" s="70"/>
-      <c r="AD9" s="70"/>
-      <c r="AE9" s="70"/>
-      <c r="AF9" s="70"/>
-      <c r="AG9" s="70" t="s">
+      <c r="R9" s="81"/>
+      <c r="S9" s="81"/>
+      <c r="T9" s="81"/>
+      <c r="U9" s="81"/>
+      <c r="V9" s="81"/>
+      <c r="W9" s="81"/>
+      <c r="X9" s="81"/>
+      <c r="Y9" s="81"/>
+      <c r="Z9" s="81"/>
+      <c r="AA9" s="81"/>
+      <c r="AB9" s="81"/>
+      <c r="AC9" s="81"/>
+      <c r="AD9" s="81"/>
+      <c r="AE9" s="81"/>
+      <c r="AF9" s="81"/>
+      <c r="AG9" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="AH9" s="70"/>
-      <c r="AI9" s="70"/>
-      <c r="AJ9" s="70"/>
-      <c r="AK9" s="70"/>
-      <c r="AL9" s="70"/>
-      <c r="AM9" s="70"/>
-      <c r="AN9" s="70"/>
-      <c r="AO9" s="70" t="s">
+      <c r="AH9" s="81"/>
+      <c r="AI9" s="81"/>
+      <c r="AJ9" s="81"/>
+      <c r="AK9" s="81"/>
+      <c r="AL9" s="81"/>
+      <c r="AM9" s="81"/>
+      <c r="AN9" s="81"/>
+      <c r="AO9" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="AP9" s="70"/>
-      <c r="AQ9" s="70"/>
-      <c r="AR9" s="70"/>
-      <c r="AS9" s="70"/>
-      <c r="AT9" s="70"/>
-      <c r="AU9" s="70"/>
-      <c r="AV9" s="71"/>
+      <c r="AP9" s="81"/>
+      <c r="AQ9" s="81"/>
+      <c r="AR9" s="81"/>
+      <c r="AS9" s="81"/>
+      <c r="AT9" s="81"/>
+      <c r="AU9" s="81"/>
+      <c r="AV9" s="89"/>
     </row>
     <row r="10" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="64"/>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="75"/>
+      <c r="B10" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="75"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="76"/>
-      <c r="L10" s="76"/>
-      <c r="M10" s="76"/>
-      <c r="N10" s="76"/>
-      <c r="O10" s="76"/>
-      <c r="P10" s="77"/>
-      <c r="Q10" s="70" t="s">
+      <c r="H10" s="93"/>
+      <c r="I10" s="94"/>
+      <c r="J10" s="94"/>
+      <c r="K10" s="94"/>
+      <c r="L10" s="94"/>
+      <c r="M10" s="94"/>
+      <c r="N10" s="94"/>
+      <c r="O10" s="94"/>
+      <c r="P10" s="95"/>
+      <c r="Q10" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="R10" s="70"/>
-      <c r="S10" s="70"/>
-      <c r="T10" s="70"/>
-      <c r="U10" s="70"/>
-      <c r="V10" s="70"/>
-      <c r="W10" s="70"/>
-      <c r="X10" s="70"/>
-      <c r="Y10" s="70"/>
-      <c r="Z10" s="70"/>
-      <c r="AA10" s="70"/>
-      <c r="AB10" s="70"/>
-      <c r="AC10" s="70"/>
-      <c r="AD10" s="70"/>
-      <c r="AE10" s="70"/>
-      <c r="AF10" s="70"/>
-      <c r="AG10" s="70" t="s">
+      <c r="R10" s="81"/>
+      <c r="S10" s="81"/>
+      <c r="T10" s="81"/>
+      <c r="U10" s="81"/>
+      <c r="V10" s="81"/>
+      <c r="W10" s="81"/>
+      <c r="X10" s="81"/>
+      <c r="Y10" s="81"/>
+      <c r="Z10" s="81"/>
+      <c r="AA10" s="81"/>
+      <c r="AB10" s="81"/>
+      <c r="AC10" s="81"/>
+      <c r="AD10" s="81"/>
+      <c r="AE10" s="81"/>
+      <c r="AF10" s="81"/>
+      <c r="AG10" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="AH10" s="70"/>
-      <c r="AI10" s="70"/>
-      <c r="AJ10" s="70"/>
-      <c r="AK10" s="70"/>
-      <c r="AL10" s="70"/>
-      <c r="AM10" s="70"/>
-      <c r="AN10" s="70"/>
-      <c r="AO10" s="70" t="s">
+      <c r="AH10" s="81"/>
+      <c r="AI10" s="81"/>
+      <c r="AJ10" s="81"/>
+      <c r="AK10" s="81"/>
+      <c r="AL10" s="81"/>
+      <c r="AM10" s="81"/>
+      <c r="AN10" s="81"/>
+      <c r="AO10" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="AP10" s="70"/>
-      <c r="AQ10" s="70"/>
-      <c r="AR10" s="70"/>
-      <c r="AS10" s="70"/>
-      <c r="AT10" s="70"/>
-      <c r="AU10" s="70"/>
-      <c r="AV10" s="71"/>
+      <c r="AP10" s="81"/>
+      <c r="AQ10" s="81"/>
+      <c r="AR10" s="81"/>
+      <c r="AS10" s="81"/>
+      <c r="AT10" s="81"/>
+      <c r="AU10" s="81"/>
+      <c r="AV10" s="89"/>
     </row>
     <row r="11" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="87"/>
+      <c r="D11" s="88"/>
     </row>
     <row r="12" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="64"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="75"/>
+      <c r="B12" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="97" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="79" t="s">
+      <c r="B13" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="79"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="79"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
-      <c r="N13" s="79"/>
-      <c r="O13" s="79"/>
-      <c r="P13" s="80"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="87"/>
+      <c r="L13" s="87"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="87"/>
+      <c r="O13" s="87"/>
+      <c r="P13" s="88"/>
     </row>
     <row r="14" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="82"/>
-      <c r="B14" s="15" t="s">
+      <c r="A14" s="98"/>
+      <c r="B14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="I14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="J14" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L14" s="15" t="s">
+      <c r="L14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M14" s="15" t="s">
+      <c r="M14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="N14" s="15" t="s">
+      <c r="N14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O14" s="15" t="s">
+      <c r="O14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="P14" s="16" t="s">
+      <c r="P14" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="79" t="s">
+      <c r="B15" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="80"/>
-      <c r="AX15" s="88"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="88"/>
+      <c r="AX15" s="26"/>
     </row>
     <row r="16" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="64"/>
-      <c r="B16" s="21" t="s">
+      <c r="A16" s="75"/>
+      <c r="B16" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="AX16" s="88"/>
+      <c r="AX16" s="26"/>
     </row>
     <row r="17" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="66"/>
-      <c r="AX17" s="88"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="76"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="76"/>
+      <c r="L17" s="76"/>
+      <c r="M17" s="77"/>
+      <c r="AX17" s="26"/>
     </row>
     <row r="18" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="64"/>
-      <c r="B18" s="19" t="s">
+      <c r="A18" s="75"/>
+      <c r="B18" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F18" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="19" t="s">
+      <c r="K18" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="L18" s="19" t="s">
+      <c r="L18" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="M18" s="20" t="s">
+      <c r="M18" s="19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="64" t="s">
+      <c r="A19" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="65" t="s">
+      <c r="B19" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="66"/>
+      <c r="C19" s="77"/>
     </row>
     <row r="20" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="64"/>
-      <c r="B20" s="19" t="s">
+      <c r="A20" s="75"/>
+      <c r="B20" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="25" t="s">
         <v>68</v>
       </c>
+    </row>
+    <row r="21" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="103" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="76"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="76"/>
+      <c r="L21" s="76"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="76"/>
+      <c r="O21" s="76"/>
+      <c r="P21" s="76"/>
+      <c r="Q21" s="76"/>
+      <c r="R21" s="76"/>
+      <c r="S21" s="76"/>
+      <c r="T21" s="76"/>
+      <c r="U21" s="76"/>
+      <c r="V21" s="76"/>
+      <c r="W21" s="76"/>
+      <c r="X21" s="76"/>
+      <c r="Y21" s="76"/>
+      <c r="Z21" s="76"/>
+      <c r="AA21" s="76"/>
+      <c r="AB21" s="76"/>
+      <c r="AC21" s="76"/>
+      <c r="AD21" s="76"/>
+      <c r="AE21" s="76"/>
+      <c r="AF21" s="76"/>
+      <c r="AG21" s="77"/>
+    </row>
+    <row r="22" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="75"/>
+      <c r="B22" s="96" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="76"/>
+      <c r="L22" s="76"/>
+      <c r="M22" s="76"/>
+      <c r="N22" s="76"/>
+      <c r="O22" s="76"/>
+      <c r="P22" s="76"/>
+      <c r="Q22" s="76"/>
+      <c r="R22" s="76"/>
+      <c r="S22" s="76"/>
+      <c r="T22" s="76"/>
+      <c r="U22" s="76"/>
+      <c r="V22" s="76"/>
+      <c r="W22" s="76"/>
+      <c r="X22" s="76"/>
+      <c r="Y22" s="76"/>
+      <c r="Z22" s="76"/>
+      <c r="AA22" s="76"/>
+      <c r="AB22" s="76"/>
+      <c r="AC22" s="76"/>
+      <c r="AD22" s="76"/>
+      <c r="AE22" s="76"/>
+      <c r="AF22" s="76"/>
+      <c r="AG22" s="77"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="34">
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:AG21"/>
+    <mergeCell ref="B22:AG22"/>
     <mergeCell ref="AO9:AV9"/>
     <mergeCell ref="AO10:AV10"/>
     <mergeCell ref="K3:P4"/>

</xml_diff>

<commit_message>
Message decoding module is beta version
</commit_message>
<xml_diff>
--- a/FileTransporter/Models/Documents/Protocol commands specification.xlsx
+++ b/FileTransporter/Models/Documents/Protocol commands specification.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\FileTransporter\FileTransporter\Models\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B917C1A-1EFA-433E-AE95-7223B395F25D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="12240" tabRatio="245" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commands for client" sheetId="1" r:id="rId1"/>
@@ -15,17 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="74">
   <si>
     <t>List of commands for client</t>
   </si>
@@ -244,12 +245,15 @@
   </si>
   <si>
     <t>10.</t>
+  </si>
+  <si>
+    <t>0x0 32 times</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;"/>
   </numFmts>
@@ -414,7 +418,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -952,6 +956,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -972,7 +989,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1056,6 +1073,24 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1065,36 +1100,114 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1104,105 +1217,63 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="21" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="26" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="22" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="29" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1212,9 +1283,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="29" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1230,67 +1298,22 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="20" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="26" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="22" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="47" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="10 % - Akcent 6" xfId="10"/>
-    <cellStyle name="10% - Akcent 1" xfId="4"/>
-    <cellStyle name="20% - akcent 1" xfId="2" builtinId="30"/>
-    <cellStyle name="20% - akcent 6" xfId="7" builtinId="50"/>
-    <cellStyle name="40% - akcent 1" xfId="3" builtinId="31"/>
-    <cellStyle name="40% - akcent 6" xfId="8" builtinId="51"/>
-    <cellStyle name="5% - Akcent 1" xfId="5"/>
-    <cellStyle name="60% - akcent 6" xfId="9" builtinId="52"/>
+    <cellStyle name="10 % - Akcent 6" xfId="10" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="10% - Akcent 1" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% — akcent 1" xfId="2" builtinId="30"/>
+    <cellStyle name="20% — akcent 6" xfId="7" builtinId="50"/>
+    <cellStyle name="40% — akcent 1" xfId="3" builtinId="31"/>
+    <cellStyle name="40% — akcent 6" xfId="8" builtinId="51"/>
+    <cellStyle name="5% - Akcent 1" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="60% — akcent 6" xfId="9" builtinId="52"/>
     <cellStyle name="Nagłówek 1" xfId="1" builtinId="16"/>
     <cellStyle name="Nagłówek 2" xfId="6" builtinId="17"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1608,236 +1631,236 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EI16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:AG16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:139" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="71"/>
-      <c r="X1" s="71"/>
-      <c r="Y1" s="71"/>
-      <c r="Z1" s="71"/>
-      <c r="AA1" s="71"/>
-      <c r="AB1" s="71"/>
-      <c r="AC1" s="71"/>
-      <c r="AD1" s="71"/>
-      <c r="AE1" s="71"/>
-      <c r="AF1" s="71"/>
-      <c r="AG1" s="71"/>
-      <c r="AH1" s="71"/>
-      <c r="AI1" s="71"/>
-      <c r="AJ1" s="71"/>
-      <c r="AK1" s="71"/>
-      <c r="AL1" s="71"/>
-      <c r="AM1" s="71"/>
-      <c r="AN1" s="71"/>
-      <c r="AO1" s="71"/>
-      <c r="AP1" s="71"/>
-      <c r="AQ1" s="71"/>
-      <c r="AR1" s="71"/>
-      <c r="AS1" s="71"/>
-      <c r="AT1" s="71"/>
-      <c r="AU1" s="71"/>
-      <c r="AV1" s="71"/>
-      <c r="AW1" s="71"/>
-      <c r="AX1" s="71"/>
-      <c r="AY1" s="71"/>
-      <c r="AZ1" s="71"/>
-      <c r="BA1" s="71"/>
-      <c r="BB1" s="71"/>
-      <c r="BC1" s="71"/>
-      <c r="BD1" s="71"/>
-      <c r="BE1" s="71"/>
-      <c r="BF1" s="71"/>
-      <c r="BG1" s="71"/>
-      <c r="BH1" s="71"/>
-      <c r="BI1" s="71"/>
-      <c r="BJ1" s="71"/>
-      <c r="BK1" s="71"/>
-      <c r="BL1" s="71"/>
-      <c r="BM1" s="71"/>
-      <c r="BN1" s="71"/>
-      <c r="BO1" s="71"/>
-      <c r="BP1" s="71"/>
-      <c r="BQ1" s="71"/>
-      <c r="BR1" s="71"/>
-      <c r="BS1" s="71"/>
-      <c r="BT1" s="71"/>
-      <c r="BU1" s="71"/>
-      <c r="BV1" s="71"/>
-      <c r="BW1" s="71"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
+      <c r="AW1" s="46"/>
+      <c r="AX1" s="46"/>
+      <c r="AY1" s="46"/>
+      <c r="AZ1" s="46"/>
+      <c r="BA1" s="46"/>
+      <c r="BB1" s="46"/>
+      <c r="BC1" s="46"/>
+      <c r="BD1" s="46"/>
+      <c r="BE1" s="46"/>
+      <c r="BF1" s="46"/>
+      <c r="BG1" s="46"/>
+      <c r="BH1" s="46"/>
+      <c r="BI1" s="46"/>
+      <c r="BJ1" s="46"/>
+      <c r="BK1" s="46"/>
+      <c r="BL1" s="46"/>
+      <c r="BM1" s="46"/>
+      <c r="BN1" s="46"/>
+      <c r="BO1" s="46"/>
+      <c r="BP1" s="46"/>
+      <c r="BQ1" s="46"/>
+      <c r="BR1" s="46"/>
+      <c r="BS1" s="46"/>
+      <c r="BT1" s="46"/>
+      <c r="BU1" s="46"/>
+      <c r="BV1" s="46"/>
+      <c r="BW1" s="46"/>
     </row>
     <row r="2" spans="1:139" s="27" customFormat="1" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="63" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="64"/>
-      <c r="U2" s="64"/>
-      <c r="V2" s="64"/>
-      <c r="W2" s="64"/>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="64"/>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="64"/>
-      <c r="AC2" s="64"/>
-      <c r="AD2" s="64"/>
-      <c r="AE2" s="64"/>
-      <c r="AF2" s="64"/>
-      <c r="AG2" s="64"/>
-      <c r="AH2" s="64"/>
-      <c r="AI2" s="64"/>
-      <c r="AJ2" s="64"/>
-      <c r="AK2" s="64"/>
-      <c r="AL2" s="64"/>
-      <c r="AM2" s="64"/>
-      <c r="AN2" s="64"/>
-      <c r="AO2" s="64"/>
-      <c r="AP2" s="64"/>
-      <c r="AQ2" s="64"/>
-      <c r="AR2" s="64"/>
-      <c r="AS2" s="64"/>
-      <c r="AT2" s="64"/>
-      <c r="AU2" s="64"/>
-      <c r="AV2" s="64"/>
-      <c r="AW2" s="64"/>
-      <c r="AX2" s="64"/>
-      <c r="AY2" s="64"/>
-      <c r="AZ2" s="64"/>
-      <c r="BA2" s="64"/>
-      <c r="BB2" s="64"/>
-      <c r="BC2" s="64"/>
-      <c r="BD2" s="64"/>
-      <c r="BE2" s="64"/>
-      <c r="BF2" s="64"/>
-      <c r="BG2" s="64"/>
-      <c r="BH2" s="64"/>
-      <c r="BI2" s="64"/>
-      <c r="BJ2" s="64"/>
-      <c r="BK2" s="64"/>
-      <c r="BL2" s="64"/>
-      <c r="BM2" s="64"/>
-      <c r="BN2" s="64"/>
-      <c r="BO2" s="64"/>
-      <c r="BP2" s="64"/>
-      <c r="BQ2" s="64"/>
-      <c r="BR2" s="64"/>
-      <c r="BS2" s="64"/>
-      <c r="BT2" s="64"/>
-      <c r="BU2" s="64"/>
-      <c r="BV2" s="64"/>
-      <c r="BW2" s="65"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="39"/>
+      <c r="AI2" s="39"/>
+      <c r="AJ2" s="39"/>
+      <c r="AK2" s="39"/>
+      <c r="AL2" s="39"/>
+      <c r="AM2" s="39"/>
+      <c r="AN2" s="39"/>
+      <c r="AO2" s="39"/>
+      <c r="AP2" s="39"/>
+      <c r="AQ2" s="39"/>
+      <c r="AR2" s="39"/>
+      <c r="AS2" s="39"/>
+      <c r="AT2" s="39"/>
+      <c r="AU2" s="39"/>
+      <c r="AV2" s="39"/>
+      <c r="AW2" s="39"/>
+      <c r="AX2" s="39"/>
+      <c r="AY2" s="39"/>
+      <c r="AZ2" s="39"/>
+      <c r="BA2" s="39"/>
+      <c r="BB2" s="39"/>
+      <c r="BC2" s="39"/>
+      <c r="BD2" s="39"/>
+      <c r="BE2" s="39"/>
+      <c r="BF2" s="39"/>
+      <c r="BG2" s="39"/>
+      <c r="BH2" s="39"/>
+      <c r="BI2" s="39"/>
+      <c r="BJ2" s="39"/>
+      <c r="BK2" s="39"/>
+      <c r="BL2" s="39"/>
+      <c r="BM2" s="39"/>
+      <c r="BN2" s="39"/>
+      <c r="BO2" s="39"/>
+      <c r="BP2" s="39"/>
+      <c r="BQ2" s="39"/>
+      <c r="BR2" s="39"/>
+      <c r="BS2" s="39"/>
+      <c r="BT2" s="39"/>
+      <c r="BU2" s="39"/>
+      <c r="BV2" s="39"/>
+      <c r="BW2" s="40"/>
     </row>
     <row r="3" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="48" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49" t="s">
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="49"/>
-      <c r="S3" s="49"/>
-      <c r="T3" s="49"/>
-      <c r="U3" s="49"/>
-      <c r="V3" s="49"/>
-      <c r="W3" s="49"/>
-      <c r="X3" s="49"/>
-      <c r="Y3" s="49"/>
-      <c r="Z3" s="49" t="s">
+      <c r="R3" s="62"/>
+      <c r="S3" s="62"/>
+      <c r="T3" s="62"/>
+      <c r="U3" s="62"/>
+      <c r="V3" s="62"/>
+      <c r="W3" s="62"/>
+      <c r="X3" s="62"/>
+      <c r="Y3" s="62"/>
+      <c r="Z3" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="AA3" s="49"/>
-      <c r="AB3" s="49"/>
-      <c r="AC3" s="49"/>
-      <c r="AD3" s="49"/>
-      <c r="AE3" s="49"/>
-      <c r="AF3" s="49" t="s">
+      <c r="AA3" s="62"/>
+      <c r="AB3" s="62"/>
+      <c r="AC3" s="62"/>
+      <c r="AD3" s="62"/>
+      <c r="AE3" s="62"/>
+      <c r="AF3" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="AG3" s="49"/>
-      <c r="AH3" s="49"/>
-      <c r="AI3" s="49"/>
-      <c r="AJ3" s="49"/>
-      <c r="AK3" s="49"/>
-      <c r="AL3" s="49"/>
-      <c r="AM3" s="56"/>
+      <c r="AG3" s="62"/>
+      <c r="AH3" s="62"/>
+      <c r="AI3" s="62"/>
+      <c r="AJ3" s="62"/>
+      <c r="AK3" s="62"/>
+      <c r="AL3" s="62"/>
+      <c r="AM3" s="64"/>
       <c r="AN3" s="3"/>
       <c r="AO3" s="3"/>
       <c r="AP3" s="3"/>
@@ -1874,7 +1897,7 @@
       <c r="BU3" s="3"/>
     </row>
     <row r="4" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="23" t="s">
         <v>10</v>
       </c>
@@ -1893,10 +1916,10 @@
       <c r="G4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="61"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="62"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="70"/>
       <c r="L4" s="12" t="s">
         <v>16</v>
       </c>
@@ -1909,20 +1932,20 @@
       <c r="O4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="99" t="s">
+      <c r="P4" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="Q4" s="50" t="s">
+      <c r="Q4" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="R4" s="50"/>
-      <c r="S4" s="50"/>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50"/>
-      <c r="V4" s="50"/>
-      <c r="W4" s="50"/>
-      <c r="X4" s="50"/>
-      <c r="Y4" s="50"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="63"/>
+      <c r="V4" s="63"/>
+      <c r="W4" s="63"/>
+      <c r="X4" s="63"/>
+      <c r="Y4" s="63"/>
       <c r="Z4" s="9" t="s">
         <v>15</v>
       </c>
@@ -1938,19 +1961,19 @@
       <c r="AD4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AE4" s="99" t="s">
+      <c r="AE4" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="AF4" s="50" t="s">
+      <c r="AF4" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="AG4" s="50"/>
-      <c r="AH4" s="50"/>
-      <c r="AI4" s="50"/>
-      <c r="AJ4" s="50"/>
-      <c r="AK4" s="50"/>
-      <c r="AL4" s="50"/>
-      <c r="AM4" s="57"/>
+      <c r="AG4" s="63"/>
+      <c r="AH4" s="63"/>
+      <c r="AI4" s="63"/>
+      <c r="AJ4" s="63"/>
+      <c r="AK4" s="63"/>
+      <c r="AL4" s="63"/>
+      <c r="AM4" s="65"/>
       <c r="AN4" s="5"/>
       <c r="AO4" s="5"/>
       <c r="AP4" s="3"/>
@@ -1987,71 +2010,71 @@
       <c r="BU4" s="3"/>
     </row>
     <row r="5" spans="1:139" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="38" t="s">
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
-      <c r="W5" s="38"/>
-      <c r="X5" s="38"/>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
-      <c r="AA5" s="38"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="34"/>
+      <c r="AA5" s="34"/>
       <c r="AB5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="AC5" s="38" t="s">
+      <c r="AC5" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="AD5" s="38"/>
-      <c r="AE5" s="38"/>
-      <c r="AF5" s="38"/>
-      <c r="AG5" s="38"/>
-      <c r="AH5" s="38"/>
-      <c r="AI5" s="38"/>
-      <c r="AJ5" s="38"/>
-      <c r="AK5" s="38"/>
-      <c r="AL5" s="38"/>
-      <c r="AM5" s="36" t="s">
+      <c r="AD5" s="34"/>
+      <c r="AE5" s="34"/>
+      <c r="AF5" s="34"/>
+      <c r="AG5" s="34"/>
+      <c r="AH5" s="34"/>
+      <c r="AI5" s="34"/>
+      <c r="AJ5" s="34"/>
+      <c r="AK5" s="34"/>
+      <c r="AL5" s="34"/>
+      <c r="AM5" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="AN5" s="37"/>
-      <c r="AO5" s="39" t="s">
+      <c r="AN5" s="73"/>
+      <c r="AO5" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="AP5" s="40"/>
-      <c r="AQ5" s="40"/>
-      <c r="AR5" s="40"/>
-      <c r="AS5" s="40"/>
-      <c r="AT5" s="40"/>
-      <c r="AU5" s="40"/>
-      <c r="AV5" s="41"/>
+      <c r="AP5" s="32"/>
+      <c r="AQ5" s="32"/>
+      <c r="AR5" s="32"/>
+      <c r="AS5" s="32"/>
+      <c r="AT5" s="32"/>
+      <c r="AU5" s="32"/>
+      <c r="AV5" s="33"/>
     </row>
     <row r="6" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="7" t="s">
         <v>26</v>
       </c>
@@ -2079,91 +2102,91 @@
       <c r="J6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="47"/>
-      <c r="L6" s="38" t="s">
+      <c r="K6" s="78"/>
+      <c r="L6" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="38"/>
-      <c r="S6" s="38"/>
-      <c r="T6" s="38"/>
-      <c r="U6" s="38"/>
-      <c r="V6" s="38"/>
-      <c r="W6" s="38"/>
-      <c r="X6" s="38"/>
-      <c r="Y6" s="38"/>
-      <c r="Z6" s="38"/>
-      <c r="AA6" s="38"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="34"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="34"/>
+      <c r="Y6" s="34"/>
+      <c r="Z6" s="34"/>
+      <c r="AA6" s="34"/>
       <c r="AB6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AC6" s="38" t="s">
+      <c r="AC6" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="AD6" s="38"/>
-      <c r="AE6" s="38"/>
-      <c r="AF6" s="38"/>
-      <c r="AG6" s="38"/>
-      <c r="AH6" s="38"/>
-      <c r="AI6" s="38"/>
-      <c r="AJ6" s="38"/>
-      <c r="AK6" s="38"/>
-      <c r="AL6" s="38"/>
+      <c r="AD6" s="34"/>
+      <c r="AE6" s="34"/>
+      <c r="AF6" s="34"/>
+      <c r="AG6" s="34"/>
+      <c r="AH6" s="34"/>
+      <c r="AI6" s="34"/>
+      <c r="AJ6" s="34"/>
+      <c r="AK6" s="34"/>
+      <c r="AL6" s="34"/>
       <c r="AM6" s="6" t="s">
         <v>25</v>
       </c>
       <c r="AN6" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="AO6" s="39" t="s">
+      <c r="AO6" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="AP6" s="40"/>
-      <c r="AQ6" s="40"/>
-      <c r="AR6" s="40"/>
-      <c r="AS6" s="40"/>
-      <c r="AT6" s="40"/>
-      <c r="AU6" s="40"/>
-      <c r="AV6" s="41"/>
+      <c r="AP6" s="32"/>
+      <c r="AQ6" s="32"/>
+      <c r="AR6" s="32"/>
+      <c r="AS6" s="32"/>
+      <c r="AT6" s="32"/>
+      <c r="AU6" s="32"/>
+      <c r="AV6" s="33"/>
     </row>
     <row r="7" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="38" t="s">
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38"/>
-      <c r="U7" s="38"/>
-      <c r="V7" s="38"/>
-      <c r="W7" s="38"/>
-      <c r="X7" s="38"/>
-      <c r="Y7" s="38"/>
-      <c r="Z7" s="38"/>
-      <c r="AA7" s="45"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="34"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
+      <c r="V7" s="34"/>
+      <c r="W7" s="34"/>
+      <c r="X7" s="34"/>
+      <c r="Y7" s="34"/>
+      <c r="Z7" s="34"/>
+      <c r="AA7" s="49"/>
       <c r="AB7" s="4"/>
       <c r="AC7" s="4"/>
       <c r="AD7" s="4"/>
@@ -2278,7 +2301,7 @@
       <c r="EI7" s="1"/>
     </row>
     <row r="8" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="7" t="s">
         <v>49</v>
       </c>
@@ -2309,24 +2332,24 @@
       <c r="K8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="38" t="s">
+      <c r="L8" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="38"/>
-      <c r="U8" s="38"/>
-      <c r="V8" s="38"/>
-      <c r="W8" s="38"/>
-      <c r="X8" s="38"/>
-      <c r="Y8" s="38"/>
-      <c r="Z8" s="38"/>
-      <c r="AA8" s="45"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="34"/>
+      <c r="T8" s="34"/>
+      <c r="U8" s="34"/>
+      <c r="V8" s="34"/>
+      <c r="W8" s="34"/>
+      <c r="X8" s="34"/>
+      <c r="Y8" s="34"/>
+      <c r="Z8" s="34"/>
+      <c r="AA8" s="49"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
       <c r="AD8" s="4"/>
@@ -2441,104 +2464,104 @@
       <c r="EI8" s="1"/>
     </row>
     <row r="9" spans="1:139" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="39" t="s">
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="40"/>
-      <c r="S9" s="40"/>
-      <c r="T9" s="40"/>
-      <c r="U9" s="40"/>
-      <c r="V9" s="40"/>
-      <c r="W9" s="40"/>
-      <c r="X9" s="40"/>
-      <c r="Y9" s="40"/>
-      <c r="Z9" s="40"/>
-      <c r="AA9" s="73"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32"/>
+      <c r="W9" s="32"/>
+      <c r="X9" s="32"/>
+      <c r="Y9" s="32"/>
+      <c r="Z9" s="32"/>
+      <c r="AA9" s="50"/>
       <c r="AB9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AC9" s="38" t="s">
+      <c r="AC9" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="AD9" s="38"/>
-      <c r="AE9" s="38"/>
-      <c r="AF9" s="38"/>
-      <c r="AG9" s="38"/>
-      <c r="AH9" s="38"/>
-      <c r="AI9" s="38"/>
-      <c r="AJ9" s="38"/>
-      <c r="AK9" s="38" t="s">
+      <c r="AD9" s="34"/>
+      <c r="AE9" s="34"/>
+      <c r="AF9" s="34"/>
+      <c r="AG9" s="34"/>
+      <c r="AH9" s="34"/>
+      <c r="AI9" s="34"/>
+      <c r="AJ9" s="34"/>
+      <c r="AK9" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="AL9" s="38"/>
-      <c r="AM9" s="38"/>
-      <c r="AN9" s="38"/>
-      <c r="AO9" s="38"/>
-      <c r="AP9" s="38"/>
-      <c r="AQ9" s="38"/>
-      <c r="AR9" s="38"/>
+      <c r="AL9" s="34"/>
+      <c r="AM9" s="34"/>
+      <c r="AN9" s="34"/>
+      <c r="AO9" s="34"/>
+      <c r="AP9" s="34"/>
+      <c r="AQ9" s="34"/>
+      <c r="AR9" s="34"/>
       <c r="AS9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="AT9" s="38" t="s">
+      <c r="AT9" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="AU9" s="38"/>
-      <c r="AV9" s="38"/>
-      <c r="AW9" s="38"/>
-      <c r="AX9" s="38"/>
-      <c r="AY9" s="38"/>
-      <c r="AZ9" s="38"/>
-      <c r="BA9" s="38"/>
-      <c r="BB9" s="38"/>
+      <c r="AU9" s="34"/>
+      <c r="AV9" s="34"/>
+      <c r="AW9" s="34"/>
+      <c r="AX9" s="34"/>
+      <c r="AY9" s="34"/>
+      <c r="AZ9" s="34"/>
+      <c r="BA9" s="34"/>
+      <c r="BB9" s="34"/>
       <c r="BC9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="BD9" s="39" t="s">
+      <c r="BD9" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="BE9" s="40"/>
-      <c r="BF9" s="40"/>
-      <c r="BG9" s="40"/>
-      <c r="BH9" s="40"/>
-      <c r="BI9" s="40"/>
-      <c r="BJ9" s="40"/>
-      <c r="BK9" s="40"/>
-      <c r="BL9" s="40"/>
-      <c r="BM9" s="40"/>
-      <c r="BN9" s="40"/>
-      <c r="BO9" s="40"/>
-      <c r="BP9" s="40"/>
-      <c r="BQ9" s="40"/>
-      <c r="BR9" s="40"/>
-      <c r="BS9" s="40"/>
-      <c r="BT9" s="40"/>
-      <c r="BU9" s="40"/>
-      <c r="BV9" s="40"/>
-      <c r="BW9" s="41"/>
+      <c r="BE9" s="32"/>
+      <c r="BF9" s="32"/>
+      <c r="BG9" s="32"/>
+      <c r="BH9" s="32"/>
+      <c r="BI9" s="32"/>
+      <c r="BJ9" s="32"/>
+      <c r="BK9" s="32"/>
+      <c r="BL9" s="32"/>
+      <c r="BM9" s="32"/>
+      <c r="BN9" s="32"/>
+      <c r="BO9" s="32"/>
+      <c r="BP9" s="32"/>
+      <c r="BQ9" s="32"/>
+      <c r="BR9" s="32"/>
+      <c r="BS9" s="32"/>
+      <c r="BT9" s="32"/>
+      <c r="BU9" s="32"/>
+      <c r="BV9" s="32"/>
+      <c r="BW9" s="33"/>
     </row>
     <row r="10" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="7" t="s">
         <v>49</v>
       </c>
@@ -2569,121 +2592,121 @@
       <c r="K10" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="39" t="s">
+      <c r="L10" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="40"/>
-      <c r="S10" s="40"/>
-      <c r="T10" s="40"/>
-      <c r="U10" s="40"/>
-      <c r="V10" s="40"/>
-      <c r="W10" s="40"/>
-      <c r="X10" s="40"/>
-      <c r="Y10" s="40"/>
-      <c r="Z10" s="40"/>
-      <c r="AA10" s="73"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
+      <c r="X10" s="32"/>
+      <c r="Y10" s="32"/>
+      <c r="Z10" s="32"/>
+      <c r="AA10" s="50"/>
       <c r="AB10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AC10" s="38" t="s">
+      <c r="AC10" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="AD10" s="38"/>
-      <c r="AE10" s="38"/>
-      <c r="AF10" s="38"/>
-      <c r="AG10" s="38"/>
-      <c r="AH10" s="38"/>
-      <c r="AI10" s="38"/>
-      <c r="AJ10" s="38"/>
-      <c r="AK10" s="38" t="s">
+      <c r="AD10" s="34"/>
+      <c r="AE10" s="34"/>
+      <c r="AF10" s="34"/>
+      <c r="AG10" s="34"/>
+      <c r="AH10" s="34"/>
+      <c r="AI10" s="34"/>
+      <c r="AJ10" s="34"/>
+      <c r="AK10" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="AL10" s="38"/>
-      <c r="AM10" s="38"/>
-      <c r="AN10" s="38"/>
-      <c r="AO10" s="38"/>
-      <c r="AP10" s="38"/>
-      <c r="AQ10" s="38"/>
-      <c r="AR10" s="38"/>
+      <c r="AL10" s="34"/>
+      <c r="AM10" s="34"/>
+      <c r="AN10" s="34"/>
+      <c r="AO10" s="34"/>
+      <c r="AP10" s="34"/>
+      <c r="AQ10" s="34"/>
+      <c r="AR10" s="34"/>
       <c r="AS10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AT10" s="38" t="s">
+      <c r="AT10" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AU10" s="38"/>
-      <c r="AV10" s="38"/>
-      <c r="AW10" s="38"/>
-      <c r="AX10" s="38"/>
-      <c r="AY10" s="38"/>
-      <c r="AZ10" s="38"/>
-      <c r="BA10" s="38"/>
-      <c r="BB10" s="38"/>
+      <c r="AU10" s="34"/>
+      <c r="AV10" s="34"/>
+      <c r="AW10" s="34"/>
+      <c r="AX10" s="34"/>
+      <c r="AY10" s="34"/>
+      <c r="AZ10" s="34"/>
+      <c r="BA10" s="34"/>
+      <c r="BB10" s="34"/>
       <c r="BC10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="BD10" s="39" t="s">
+      <c r="BD10" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="BE10" s="40"/>
-      <c r="BF10" s="40"/>
-      <c r="BG10" s="40"/>
-      <c r="BH10" s="40"/>
-      <c r="BI10" s="40"/>
-      <c r="BJ10" s="40"/>
-      <c r="BK10" s="40"/>
-      <c r="BL10" s="40"/>
-      <c r="BM10" s="40"/>
-      <c r="BN10" s="40"/>
-      <c r="BO10" s="40"/>
-      <c r="BP10" s="40"/>
-      <c r="BQ10" s="40"/>
-      <c r="BR10" s="40"/>
-      <c r="BS10" s="40"/>
-      <c r="BT10" s="40"/>
-      <c r="BU10" s="40"/>
-      <c r="BV10" s="40"/>
-      <c r="BW10" s="41"/>
+      <c r="BE10" s="32"/>
+      <c r="BF10" s="32"/>
+      <c r="BG10" s="32"/>
+      <c r="BH10" s="32"/>
+      <c r="BI10" s="32"/>
+      <c r="BJ10" s="32"/>
+      <c r="BK10" s="32"/>
+      <c r="BL10" s="32"/>
+      <c r="BM10" s="32"/>
+      <c r="BN10" s="32"/>
+      <c r="BO10" s="32"/>
+      <c r="BP10" s="32"/>
+      <c r="BQ10" s="32"/>
+      <c r="BR10" s="32"/>
+      <c r="BS10" s="32"/>
+      <c r="BT10" s="32"/>
+      <c r="BU10" s="32"/>
+      <c r="BV10" s="32"/>
+      <c r="BW10" s="33"/>
     </row>
     <row r="11" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="38" t="s">
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="38"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="38"/>
-      <c r="X11" s="38"/>
-      <c r="Y11" s="38"/>
-      <c r="Z11" s="38"/>
-      <c r="AA11" s="45"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="34"/>
+      <c r="U11" s="34"/>
+      <c r="V11" s="34"/>
+      <c r="W11" s="34"/>
+      <c r="X11" s="34"/>
+      <c r="Y11" s="34"/>
+      <c r="Z11" s="34"/>
+      <c r="AA11" s="49"/>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
@@ -2732,7 +2755,7 @@
       <c r="BU11" s="3"/>
     </row>
     <row r="12" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
@@ -2754,27 +2777,27 @@
       <c r="H12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="33"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="38" t="s">
+      <c r="I12" s="58"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="38"/>
-      <c r="U12" s="38"/>
-      <c r="V12" s="38"/>
-      <c r="W12" s="38"/>
-      <c r="X12" s="38"/>
-      <c r="Y12" s="38"/>
-      <c r="Z12" s="38"/>
-      <c r="AA12" s="45"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="34"/>
+      <c r="U12" s="34"/>
+      <c r="V12" s="34"/>
+      <c r="W12" s="34"/>
+      <c r="X12" s="34"/>
+      <c r="Y12" s="34"/>
+      <c r="Z12" s="34"/>
+      <c r="AA12" s="49"/>
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
@@ -2823,164 +2846,253 @@
       <c r="BU12" s="3"/>
     </row>
     <row r="13" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="38" t="s">
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="38"/>
-      <c r="U13" s="38"/>
-      <c r="V13" s="38"/>
-      <c r="W13" s="38"/>
-      <c r="X13" s="38"/>
-      <c r="Y13" s="38"/>
-      <c r="Z13" s="38"/>
-      <c r="AA13" s="45"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="34"/>
+      <c r="U13" s="34"/>
+      <c r="V13" s="34"/>
+      <c r="W13" s="34"/>
+      <c r="X13" s="34"/>
+      <c r="Y13" s="34"/>
+      <c r="Z13" s="34"/>
+      <c r="AA13" s="49"/>
     </row>
     <row r="14" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="100" t="s">
+      <c r="A14" s="47"/>
+      <c r="B14" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="100" t="s">
+      <c r="C14" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="100" t="s">
+      <c r="D14" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="100" t="s">
+      <c r="E14" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="100" t="s">
+      <c r="F14" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="101" t="s">
+      <c r="G14" s="58"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="M14" s="101"/>
-      <c r="N14" s="101"/>
-      <c r="O14" s="101"/>
-      <c r="P14" s="101"/>
-      <c r="Q14" s="101"/>
-      <c r="R14" s="101"/>
-      <c r="S14" s="101"/>
-      <c r="T14" s="101"/>
-      <c r="U14" s="101"/>
-      <c r="V14" s="101"/>
-      <c r="W14" s="101"/>
-      <c r="X14" s="101"/>
-      <c r="Y14" s="101"/>
-      <c r="Z14" s="101"/>
-      <c r="AA14" s="102"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="52"/>
+      <c r="T14" s="52"/>
+      <c r="U14" s="52"/>
+      <c r="V14" s="52"/>
+      <c r="W14" s="52"/>
+      <c r="X14" s="52"/>
+      <c r="Y14" s="52"/>
+      <c r="Z14" s="52"/>
+      <c r="AA14" s="53"/>
     </row>
     <row r="15" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="30"/>
-      <c r="U15" s="30"/>
-      <c r="V15" s="30"/>
-      <c r="W15" s="30"/>
-      <c r="X15" s="30"/>
-      <c r="Y15" s="30"/>
-      <c r="Z15" s="30"/>
-      <c r="AA15" s="30"/>
-      <c r="AB15" s="30"/>
-      <c r="AC15" s="30"/>
-      <c r="AD15" s="30"/>
-      <c r="AE15" s="30"/>
-      <c r="AF15" s="30"/>
-      <c r="AG15" s="31"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="36"/>
+      <c r="U15" s="36"/>
+      <c r="V15" s="36"/>
+      <c r="W15" s="36"/>
+      <c r="X15" s="36"/>
+      <c r="Y15" s="36"/>
+      <c r="Z15" s="36"/>
+      <c r="AA15" s="36"/>
+      <c r="AB15" s="36"/>
+      <c r="AC15" s="36"/>
+      <c r="AD15" s="36"/>
+      <c r="AE15" s="36"/>
+      <c r="AF15" s="36"/>
+      <c r="AG15" s="36"/>
+      <c r="AH15" s="36"/>
+      <c r="AI15" s="36"/>
+      <c r="AJ15" s="36"/>
+      <c r="AK15" s="36"/>
+      <c r="AL15" s="36"/>
+      <c r="AM15" s="36"/>
+      <c r="AN15" s="36"/>
+      <c r="AO15" s="36"/>
+      <c r="AP15" s="36"/>
+      <c r="AQ15" s="36"/>
+      <c r="AR15" s="36"/>
+      <c r="AS15" s="36"/>
+      <c r="AT15" s="36"/>
+      <c r="AU15" s="36"/>
+      <c r="AV15" s="36"/>
+      <c r="AW15" s="36"/>
+      <c r="AX15" s="36"/>
+      <c r="AY15" s="36"/>
+      <c r="AZ15" s="36"/>
+      <c r="BA15" s="36"/>
+      <c r="BB15" s="36"/>
+      <c r="BC15" s="36"/>
+      <c r="BD15" s="36"/>
+      <c r="BE15" s="36"/>
+      <c r="BF15" s="36"/>
+      <c r="BG15" s="36"/>
+      <c r="BH15" s="36"/>
+      <c r="BI15" s="36"/>
+      <c r="BJ15" s="36"/>
+      <c r="BK15" s="36"/>
+      <c r="BL15" s="36"/>
+      <c r="BM15" s="37"/>
     </row>
     <row r="16" spans="1:139" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="29" t="s">
+      <c r="A16" s="47"/>
+      <c r="B16" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="36"/>
+      <c r="U16" s="36"/>
+      <c r="V16" s="36"/>
+      <c r="W16" s="36"/>
+      <c r="X16" s="36"/>
+      <c r="Y16" s="36"/>
+      <c r="Z16" s="36"/>
+      <c r="AA16" s="36"/>
+      <c r="AB16" s="36"/>
+      <c r="AC16" s="36"/>
+      <c r="AD16" s="36"/>
+      <c r="AE16" s="36"/>
+      <c r="AF16" s="36"/>
+      <c r="AG16" s="105"/>
+      <c r="AH16" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="30"/>
-      <c r="S16" s="30"/>
-      <c r="T16" s="30"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="30"/>
-      <c r="W16" s="30"/>
-      <c r="X16" s="30"/>
-      <c r="Y16" s="30"/>
-      <c r="Z16" s="30"/>
-      <c r="AA16" s="30"/>
-      <c r="AB16" s="30"/>
-      <c r="AC16" s="30"/>
-      <c r="AD16" s="30"/>
-      <c r="AE16" s="30"/>
-      <c r="AF16" s="30"/>
-      <c r="AG16" s="31"/>
+      <c r="AI16" s="36"/>
+      <c r="AJ16" s="36"/>
+      <c r="AK16" s="36"/>
+      <c r="AL16" s="36"/>
+      <c r="AM16" s="36"/>
+      <c r="AN16" s="36"/>
+      <c r="AO16" s="36"/>
+      <c r="AP16" s="36"/>
+      <c r="AQ16" s="36"/>
+      <c r="AR16" s="36"/>
+      <c r="AS16" s="36"/>
+      <c r="AT16" s="36"/>
+      <c r="AU16" s="36"/>
+      <c r="AV16" s="36"/>
+      <c r="AW16" s="36"/>
+      <c r="AX16" s="36"/>
+      <c r="AY16" s="36"/>
+      <c r="AZ16" s="36"/>
+      <c r="BA16" s="36"/>
+      <c r="BB16" s="36"/>
+      <c r="BC16" s="36"/>
+      <c r="BD16" s="36"/>
+      <c r="BE16" s="36"/>
+      <c r="BF16" s="36"/>
+      <c r="BG16" s="36"/>
+      <c r="BH16" s="36"/>
+      <c r="BI16" s="36"/>
+      <c r="BJ16" s="36"/>
+      <c r="BK16" s="36"/>
+      <c r="BL16" s="36"/>
+      <c r="BM16" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="BD9:BW9"/>
-    <mergeCell ref="BD10:BW10"/>
-    <mergeCell ref="AC5:AL5"/>
-    <mergeCell ref="B16:AG16"/>
-    <mergeCell ref="B15:AG15"/>
+  <mergeCells count="52">
+    <mergeCell ref="AF3:AM3"/>
+    <mergeCell ref="AF4:AM4"/>
+    <mergeCell ref="H3:K4"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="G13:K14"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AC9:AJ9"/>
+    <mergeCell ref="AC10:AJ10"/>
+    <mergeCell ref="AK9:AR9"/>
+    <mergeCell ref="AK10:AR10"/>
+    <mergeCell ref="AO5:AV5"/>
+    <mergeCell ref="AO6:AV6"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="L7:AA7"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="AC6:AL6"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="Q3:Y3"/>
+    <mergeCell ref="Q4:Y4"/>
+    <mergeCell ref="Z3:AE3"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="L11:AA11"/>
+    <mergeCell ref="L12:AA12"/>
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="I11:K12"/>
     <mergeCell ref="L2:BW2"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="B3:G3"/>
@@ -2997,36 +3109,14 @@
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="L13:AA13"/>
     <mergeCell ref="L14:AA14"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="L11:AA11"/>
-    <mergeCell ref="L12:AA12"/>
-    <mergeCell ref="B9:K9"/>
-    <mergeCell ref="I11:K12"/>
+    <mergeCell ref="BD9:BW9"/>
+    <mergeCell ref="BD10:BW10"/>
+    <mergeCell ref="AC5:AL5"/>
+    <mergeCell ref="B16:AG16"/>
     <mergeCell ref="AT10:BB10"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="Q3:Y3"/>
-    <mergeCell ref="Q4:Y4"/>
-    <mergeCell ref="Z3:AE3"/>
-    <mergeCell ref="AF3:AM3"/>
-    <mergeCell ref="AF4:AM4"/>
-    <mergeCell ref="H3:K4"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="G13:K14"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AC9:AJ9"/>
-    <mergeCell ref="AC10:AJ10"/>
-    <mergeCell ref="AK9:AR9"/>
-    <mergeCell ref="AK10:AR10"/>
-    <mergeCell ref="AO5:AV5"/>
-    <mergeCell ref="AO6:AV6"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="L7:AA7"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="AC6:AL6"/>
     <mergeCell ref="AT9:BB9"/>
+    <mergeCell ref="AH16:BM16"/>
+    <mergeCell ref="B15:BM15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3035,11 +3125,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:BM22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AG26" sqref="AG26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3050,139 +3140,139 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
-      <c r="T1" s="80"/>
-      <c r="U1" s="80"/>
-      <c r="V1" s="80"/>
-      <c r="W1" s="80"/>
-      <c r="X1" s="80"/>
-      <c r="Y1" s="80"/>
-      <c r="Z1" s="80"/>
-      <c r="AA1" s="80"/>
-      <c r="AB1" s="80"/>
-      <c r="AC1" s="80"/>
-      <c r="AD1" s="80"/>
-      <c r="AE1" s="80"/>
-      <c r="AF1" s="80"/>
-      <c r="AG1" s="80"/>
-      <c r="AH1" s="80"/>
-      <c r="AI1" s="80"/>
-      <c r="AJ1" s="80"/>
-      <c r="AK1" s="80"/>
-      <c r="AL1" s="80"/>
-      <c r="AM1" s="80"/>
-      <c r="AN1" s="80"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="98"/>
+      <c r="Y1" s="98"/>
+      <c r="Z1" s="98"/>
+      <c r="AA1" s="98"/>
+      <c r="AB1" s="98"/>
+      <c r="AC1" s="98"/>
+      <c r="AD1" s="98"/>
+      <c r="AE1" s="98"/>
+      <c r="AF1" s="98"/>
+      <c r="AG1" s="98"/>
+      <c r="AH1" s="98"/>
+      <c r="AI1" s="98"/>
+      <c r="AJ1" s="98"/>
+      <c r="AK1" s="98"/>
+      <c r="AL1" s="98"/>
+      <c r="AM1" s="98"/>
+      <c r="AN1" s="98"/>
     </row>
     <row r="2" spans="1:50" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78" t="s">
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
+      <c r="Q2" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="78"/>
-      <c r="U2" s="78"/>
-      <c r="V2" s="78"/>
-      <c r="W2" s="78"/>
-      <c r="X2" s="78"/>
-      <c r="Y2" s="78"/>
-      <c r="Z2" s="78"/>
-      <c r="AA2" s="78"/>
-      <c r="AB2" s="78"/>
-      <c r="AC2" s="78"/>
-      <c r="AD2" s="78"/>
-      <c r="AE2" s="78"/>
-      <c r="AF2" s="78"/>
-      <c r="AG2" s="78"/>
-      <c r="AH2" s="78"/>
-      <c r="AI2" s="78"/>
-      <c r="AJ2" s="78"/>
-      <c r="AK2" s="78"/>
-      <c r="AL2" s="78"/>
-      <c r="AM2" s="78"/>
-      <c r="AN2" s="78"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="96"/>
+      <c r="T2" s="96"/>
+      <c r="U2" s="96"/>
+      <c r="V2" s="96"/>
+      <c r="W2" s="96"/>
+      <c r="X2" s="96"/>
+      <c r="Y2" s="96"/>
+      <c r="Z2" s="96"/>
+      <c r="AA2" s="96"/>
+      <c r="AB2" s="96"/>
+      <c r="AC2" s="96"/>
+      <c r="AD2" s="96"/>
+      <c r="AE2" s="96"/>
+      <c r="AF2" s="96"/>
+      <c r="AG2" s="96"/>
+      <c r="AH2" s="96"/>
+      <c r="AI2" s="96"/>
+      <c r="AJ2" s="96"/>
+      <c r="AK2" s="96"/>
+      <c r="AL2" s="96"/>
+      <c r="AM2" s="96"/>
+      <c r="AN2" s="96"/>
     </row>
     <row r="3" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="83" t="s">
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="88"/>
+      <c r="Q3" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="83"/>
-      <c r="S3" s="83"/>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="83"/>
-      <c r="W3" s="83"/>
-      <c r="X3" s="83"/>
-      <c r="Y3" s="83"/>
-      <c r="Z3" s="83"/>
-      <c r="AA3" s="83"/>
-      <c r="AB3" s="83"/>
-      <c r="AC3" s="83"/>
-      <c r="AD3" s="83"/>
-      <c r="AE3" s="83"/>
-      <c r="AF3" s="84"/>
+      <c r="R3" s="100"/>
+      <c r="S3" s="100"/>
+      <c r="T3" s="100"/>
+      <c r="U3" s="100"/>
+      <c r="V3" s="100"/>
+      <c r="W3" s="100"/>
+      <c r="X3" s="100"/>
+      <c r="Y3" s="100"/>
+      <c r="Z3" s="100"/>
+      <c r="AA3" s="100"/>
+      <c r="AB3" s="100"/>
+      <c r="AC3" s="100"/>
+      <c r="AD3" s="100"/>
+      <c r="AE3" s="100"/>
+      <c r="AF3" s="101"/>
     </row>
     <row r="4" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="75"/>
+      <c r="A4" s="80"/>
       <c r="B4" s="14" t="s">
         <v>22</v>
       </c>
@@ -3210,49 +3300,49 @@
       <c r="J4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="93"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="94"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="95"/>
-      <c r="Q4" s="85" t="s">
+      <c r="K4" s="89"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="91"/>
+      <c r="Q4" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="85"/>
-      <c r="U4" s="85"/>
-      <c r="V4" s="85"/>
-      <c r="W4" s="85"/>
-      <c r="X4" s="85"/>
-      <c r="Y4" s="85"/>
-      <c r="Z4" s="85"/>
-      <c r="AA4" s="85"/>
-      <c r="AB4" s="85"/>
-      <c r="AC4" s="85"/>
-      <c r="AD4" s="85"/>
-      <c r="AE4" s="85"/>
-      <c r="AF4" s="86"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="102"/>
+      <c r="W4" s="102"/>
+      <c r="X4" s="102"/>
+      <c r="Y4" s="102"/>
+      <c r="Z4" s="102"/>
+      <c r="AA4" s="102"/>
+      <c r="AB4" s="102"/>
+      <c r="AC4" s="102"/>
+      <c r="AD4" s="102"/>
+      <c r="AE4" s="102"/>
+      <c r="AF4" s="103"/>
     </row>
     <row r="5" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="88"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="93"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="75"/>
+      <c r="A6" s="80"/>
       <c r="B6" s="14" t="s">
         <v>22</v>
       </c>
@@ -3278,23 +3368,23 @@
       <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="87" t="s">
+      <c r="B7" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="88"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="93"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="75"/>
+      <c r="A8" s="80"/>
       <c r="B8" s="14" t="s">
         <v>18</v>
       </c>
@@ -3320,67 +3410,67 @@
       <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="87" t="s">
+      <c r="B9" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
-      <c r="M9" s="94"/>
-      <c r="N9" s="94"/>
-      <c r="O9" s="94"/>
-      <c r="P9" s="95"/>
-      <c r="Q9" s="81" t="s">
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="90"/>
+      <c r="P9" s="91"/>
+      <c r="Q9" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="R9" s="81"/>
-      <c r="S9" s="81"/>
-      <c r="T9" s="81"/>
-      <c r="U9" s="81"/>
-      <c r="V9" s="81"/>
-      <c r="W9" s="81"/>
-      <c r="X9" s="81"/>
-      <c r="Y9" s="81"/>
-      <c r="Z9" s="81"/>
-      <c r="AA9" s="81"/>
-      <c r="AB9" s="81"/>
-      <c r="AC9" s="81"/>
-      <c r="AD9" s="81"/>
-      <c r="AE9" s="81"/>
-      <c r="AF9" s="81"/>
-      <c r="AG9" s="81" t="s">
+      <c r="R9" s="84"/>
+      <c r="S9" s="84"/>
+      <c r="T9" s="84"/>
+      <c r="U9" s="84"/>
+      <c r="V9" s="84"/>
+      <c r="W9" s="84"/>
+      <c r="X9" s="84"/>
+      <c r="Y9" s="84"/>
+      <c r="Z9" s="84"/>
+      <c r="AA9" s="84"/>
+      <c r="AB9" s="84"/>
+      <c r="AC9" s="84"/>
+      <c r="AD9" s="84"/>
+      <c r="AE9" s="84"/>
+      <c r="AF9" s="84"/>
+      <c r="AG9" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="AH9" s="81"/>
-      <c r="AI9" s="81"/>
-      <c r="AJ9" s="81"/>
-      <c r="AK9" s="81"/>
-      <c r="AL9" s="81"/>
-      <c r="AM9" s="81"/>
-      <c r="AN9" s="81"/>
-      <c r="AO9" s="81" t="s">
+      <c r="AH9" s="84"/>
+      <c r="AI9" s="84"/>
+      <c r="AJ9" s="84"/>
+      <c r="AK9" s="84"/>
+      <c r="AL9" s="84"/>
+      <c r="AM9" s="84"/>
+      <c r="AN9" s="84"/>
+      <c r="AO9" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="AP9" s="81"/>
-      <c r="AQ9" s="81"/>
-      <c r="AR9" s="81"/>
-      <c r="AS9" s="81"/>
-      <c r="AT9" s="81"/>
-      <c r="AU9" s="81"/>
-      <c r="AV9" s="89"/>
+      <c r="AP9" s="84"/>
+      <c r="AQ9" s="84"/>
+      <c r="AR9" s="84"/>
+      <c r="AS9" s="84"/>
+      <c r="AT9" s="84"/>
+      <c r="AU9" s="84"/>
+      <c r="AV9" s="85"/>
     </row>
     <row r="10" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="75"/>
+      <c r="A10" s="80"/>
       <c r="B10" s="14" t="s">
         <v>54</v>
       </c>
@@ -3399,66 +3489,66 @@
       <c r="G10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="93"/>
-      <c r="I10" s="94"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="94"/>
-      <c r="L10" s="94"/>
-      <c r="M10" s="94"/>
-      <c r="N10" s="94"/>
-      <c r="O10" s="94"/>
-      <c r="P10" s="95"/>
-      <c r="Q10" s="81" t="s">
+      <c r="H10" s="89"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="90"/>
+      <c r="L10" s="90"/>
+      <c r="M10" s="90"/>
+      <c r="N10" s="90"/>
+      <c r="O10" s="90"/>
+      <c r="P10" s="91"/>
+      <c r="Q10" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="R10" s="81"/>
-      <c r="S10" s="81"/>
-      <c r="T10" s="81"/>
-      <c r="U10" s="81"/>
-      <c r="V10" s="81"/>
-      <c r="W10" s="81"/>
-      <c r="X10" s="81"/>
-      <c r="Y10" s="81"/>
-      <c r="Z10" s="81"/>
-      <c r="AA10" s="81"/>
-      <c r="AB10" s="81"/>
-      <c r="AC10" s="81"/>
-      <c r="AD10" s="81"/>
-      <c r="AE10" s="81"/>
-      <c r="AF10" s="81"/>
-      <c r="AG10" s="81" t="s">
+      <c r="R10" s="84"/>
+      <c r="S10" s="84"/>
+      <c r="T10" s="84"/>
+      <c r="U10" s="84"/>
+      <c r="V10" s="84"/>
+      <c r="W10" s="84"/>
+      <c r="X10" s="84"/>
+      <c r="Y10" s="84"/>
+      <c r="Z10" s="84"/>
+      <c r="AA10" s="84"/>
+      <c r="AB10" s="84"/>
+      <c r="AC10" s="84"/>
+      <c r="AD10" s="84"/>
+      <c r="AE10" s="84"/>
+      <c r="AF10" s="84"/>
+      <c r="AG10" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="AH10" s="81"/>
-      <c r="AI10" s="81"/>
-      <c r="AJ10" s="81"/>
-      <c r="AK10" s="81"/>
-      <c r="AL10" s="81"/>
-      <c r="AM10" s="81"/>
-      <c r="AN10" s="81"/>
-      <c r="AO10" s="81" t="s">
+      <c r="AH10" s="84"/>
+      <c r="AI10" s="84"/>
+      <c r="AJ10" s="84"/>
+      <c r="AK10" s="84"/>
+      <c r="AL10" s="84"/>
+      <c r="AM10" s="84"/>
+      <c r="AN10" s="84"/>
+      <c r="AO10" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="AP10" s="81"/>
-      <c r="AQ10" s="81"/>
-      <c r="AR10" s="81"/>
-      <c r="AS10" s="81"/>
-      <c r="AT10" s="81"/>
-      <c r="AU10" s="81"/>
-      <c r="AV10" s="89"/>
+      <c r="AP10" s="84"/>
+      <c r="AQ10" s="84"/>
+      <c r="AR10" s="84"/>
+      <c r="AS10" s="84"/>
+      <c r="AT10" s="84"/>
+      <c r="AU10" s="84"/>
+      <c r="AV10" s="85"/>
     </row>
     <row r="11" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="87"/>
-      <c r="D11" s="88"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="93"/>
     </row>
     <row r="12" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="75"/>
+      <c r="A12" s="80"/>
       <c r="B12" s="20" t="s">
         <v>53</v>
       </c>
@@ -3470,29 +3560,29 @@
       </c>
     </row>
     <row r="13" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="92" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="87"/>
-      <c r="K13" s="87"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="87"/>
-      <c r="O13" s="87"/>
-      <c r="P13" s="88"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="92"/>
+      <c r="E13" s="92"/>
+      <c r="F13" s="92"/>
+      <c r="G13" s="92"/>
+      <c r="H13" s="92"/>
+      <c r="I13" s="92"/>
+      <c r="J13" s="92"/>
+      <c r="K13" s="92"/>
+      <c r="L13" s="92"/>
+      <c r="M13" s="92"/>
+      <c r="N13" s="92"/>
+      <c r="O13" s="92"/>
+      <c r="P13" s="93"/>
     </row>
     <row r="14" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="98"/>
+      <c r="A14" s="95"/>
       <c r="B14" s="14" t="s">
         <v>13</v>
       </c>
@@ -3540,22 +3630,22 @@
       </c>
     </row>
     <row r="15" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="75" t="s">
+      <c r="A15" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="87" t="s">
+      <c r="B15" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="87"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="88"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="92"/>
+      <c r="H15" s="93"/>
       <c r="AX15" s="26"/>
     </row>
     <row r="16" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="75"/>
+      <c r="A16" s="80"/>
       <c r="B16" s="20" t="s">
         <v>61</v>
       </c>
@@ -3579,28 +3669,28 @@
       </c>
       <c r="AX16" s="26"/>
     </row>
-    <row r="17" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="75" t="s">
+    <row r="17" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="96" t="s">
+      <c r="B17" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="76"/>
-      <c r="K17" s="76"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="77"/>
+      <c r="C17" s="82"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="82"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="83"/>
       <c r="AX17" s="26"/>
     </row>
-    <row r="18" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="75"/>
+    <row r="18" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="80"/>
       <c r="B18" s="18" t="s">
         <v>13</v>
       </c>
@@ -3638,17 +3728,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="75" t="s">
+    <row r="19" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="76" t="s">
+      <c r="B19" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="77"/>
+      <c r="C19" s="83"/>
     </row>
-    <row r="20" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="75"/>
+    <row r="20" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="80"/>
       <c r="B20" s="18" t="s">
         <v>11</v>
       </c>
@@ -3656,105 +3746,150 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="103" t="s">
+    <row r="21" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="96" t="s">
+      <c r="B21" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="76"/>
-      <c r="G21" s="76"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="76"/>
-      <c r="J21" s="76"/>
-      <c r="K21" s="76"/>
-      <c r="L21" s="76"/>
-      <c r="M21" s="76"/>
-      <c r="N21" s="76"/>
-      <c r="O21" s="76"/>
-      <c r="P21" s="76"/>
-      <c r="Q21" s="76"/>
-      <c r="R21" s="76"/>
-      <c r="S21" s="76"/>
-      <c r="T21" s="76"/>
-      <c r="U21" s="76"/>
-      <c r="V21" s="76"/>
-      <c r="W21" s="76"/>
-      <c r="X21" s="76"/>
-      <c r="Y21" s="76"/>
-      <c r="Z21" s="76"/>
-      <c r="AA21" s="76"/>
-      <c r="AB21" s="76"/>
-      <c r="AC21" s="76"/>
-      <c r="AD21" s="76"/>
-      <c r="AE21" s="76"/>
-      <c r="AF21" s="76"/>
-      <c r="AG21" s="77"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="82"/>
+      <c r="G21" s="82"/>
+      <c r="H21" s="82"/>
+      <c r="I21" s="82"/>
+      <c r="J21" s="82"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="82"/>
+      <c r="N21" s="82"/>
+      <c r="O21" s="82"/>
+      <c r="P21" s="82"/>
+      <c r="Q21" s="82"/>
+      <c r="R21" s="82"/>
+      <c r="S21" s="82"/>
+      <c r="T21" s="82"/>
+      <c r="U21" s="82"/>
+      <c r="V21" s="82"/>
+      <c r="W21" s="82"/>
+      <c r="X21" s="82"/>
+      <c r="Y21" s="82"/>
+      <c r="Z21" s="82"/>
+      <c r="AA21" s="82"/>
+      <c r="AB21" s="82"/>
+      <c r="AC21" s="82"/>
+      <c r="AD21" s="82"/>
+      <c r="AE21" s="82"/>
+      <c r="AF21" s="82"/>
+      <c r="AG21" s="82"/>
+      <c r="AH21" s="82"/>
+      <c r="AI21" s="82"/>
+      <c r="AJ21" s="82"/>
+      <c r="AK21" s="82"/>
+      <c r="AL21" s="82"/>
+      <c r="AM21" s="82"/>
+      <c r="AN21" s="82"/>
+      <c r="AO21" s="82"/>
+      <c r="AP21" s="82"/>
+      <c r="AQ21" s="82"/>
+      <c r="AR21" s="82"/>
+      <c r="AS21" s="82"/>
+      <c r="AT21" s="82"/>
+      <c r="AU21" s="82"/>
+      <c r="AV21" s="82"/>
+      <c r="AW21" s="82"/>
+      <c r="AX21" s="82"/>
+      <c r="AY21" s="82"/>
+      <c r="AZ21" s="82"/>
+      <c r="BA21" s="82"/>
+      <c r="BB21" s="82"/>
+      <c r="BC21" s="82"/>
+      <c r="BD21" s="82"/>
+      <c r="BE21" s="82"/>
+      <c r="BF21" s="82"/>
+      <c r="BG21" s="82"/>
+      <c r="BH21" s="82"/>
+      <c r="BI21" s="82"/>
+      <c r="BJ21" s="82"/>
+      <c r="BK21" s="82"/>
+      <c r="BL21" s="82"/>
+      <c r="BM21" s="83"/>
     </row>
-    <row r="22" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="75"/>
-      <c r="B22" s="96" t="s">
+    <row r="22" spans="1:65" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="80"/>
+      <c r="B22" s="81" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="82"/>
+      <c r="O22" s="82"/>
+      <c r="P22" s="82"/>
+      <c r="Q22" s="82"/>
+      <c r="R22" s="82"/>
+      <c r="S22" s="82"/>
+      <c r="T22" s="82"/>
+      <c r="U22" s="82"/>
+      <c r="V22" s="82"/>
+      <c r="W22" s="82"/>
+      <c r="X22" s="82"/>
+      <c r="Y22" s="82"/>
+      <c r="Z22" s="82"/>
+      <c r="AA22" s="82"/>
+      <c r="AB22" s="82"/>
+      <c r="AC22" s="82"/>
+      <c r="AD22" s="82"/>
+      <c r="AE22" s="82"/>
+      <c r="AF22" s="82"/>
+      <c r="AG22" s="104"/>
+      <c r="AH22" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="76"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="76"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="76"/>
-      <c r="J22" s="76"/>
-      <c r="K22" s="76"/>
-      <c r="L22" s="76"/>
-      <c r="M22" s="76"/>
-      <c r="N22" s="76"/>
-      <c r="O22" s="76"/>
-      <c r="P22" s="76"/>
-      <c r="Q22" s="76"/>
-      <c r="R22" s="76"/>
-      <c r="S22" s="76"/>
-      <c r="T22" s="76"/>
-      <c r="U22" s="76"/>
-      <c r="V22" s="76"/>
-      <c r="W22" s="76"/>
-      <c r="X22" s="76"/>
-      <c r="Y22" s="76"/>
-      <c r="Z22" s="76"/>
-      <c r="AA22" s="76"/>
-      <c r="AB22" s="76"/>
-      <c r="AC22" s="76"/>
-      <c r="AD22" s="76"/>
-      <c r="AE22" s="76"/>
-      <c r="AF22" s="76"/>
-      <c r="AG22" s="77"/>
+      <c r="AI22" s="82"/>
+      <c r="AJ22" s="82"/>
+      <c r="AK22" s="82"/>
+      <c r="AL22" s="82"/>
+      <c r="AM22" s="82"/>
+      <c r="AN22" s="82"/>
+      <c r="AO22" s="82"/>
+      <c r="AP22" s="82"/>
+      <c r="AQ22" s="82"/>
+      <c r="AR22" s="82"/>
+      <c r="AS22" s="82"/>
+      <c r="AT22" s="82"/>
+      <c r="AU22" s="82"/>
+      <c r="AV22" s="82"/>
+      <c r="AW22" s="82"/>
+      <c r="AX22" s="82"/>
+      <c r="AY22" s="82"/>
+      <c r="AZ22" s="82"/>
+      <c r="BA22" s="82"/>
+      <c r="BB22" s="82"/>
+      <c r="BC22" s="82"/>
+      <c r="BD22" s="82"/>
+      <c r="BE22" s="82"/>
+      <c r="BF22" s="82"/>
+      <c r="BG22" s="82"/>
+      <c r="BH22" s="82"/>
+      <c r="BI22" s="82"/>
+      <c r="BJ22" s="82"/>
+      <c r="BK22" s="82"/>
+      <c r="BL22" s="82"/>
+      <c r="BM22" s="83"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:AG21"/>
-    <mergeCell ref="B22:AG22"/>
-    <mergeCell ref="AO9:AV9"/>
-    <mergeCell ref="AO10:AV10"/>
-    <mergeCell ref="K3:P4"/>
-    <mergeCell ref="H9:P10"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="Q9:AF9"/>
-    <mergeCell ref="Q10:AF10"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:P13"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:C19"/>
+  <mergeCells count="35">
     <mergeCell ref="Q2:AN2"/>
     <mergeCell ref="A1:AN1"/>
     <mergeCell ref="AG9:AN9"/>
@@ -3768,6 +3903,28 @@
     <mergeCell ref="Q4:AF4"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B5:H5"/>
+    <mergeCell ref="K3:P4"/>
+    <mergeCell ref="H9:P10"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:P13"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B22:AG22"/>
+    <mergeCell ref="AO9:AV9"/>
+    <mergeCell ref="AO10:AV10"/>
+    <mergeCell ref="Q9:AF9"/>
+    <mergeCell ref="Q10:AF10"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="AH22:BM22"/>
+    <mergeCell ref="B21:BM21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>